<commit_message>
Updates to doc and requirements
</commit_message>
<xml_diff>
--- a/Requirements/Requirements.xlsx
+++ b/Requirements/Requirements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="100" windowWidth="27400" windowHeight="16480" tabRatio="500"/>
+    <workbookView xWindow="680" yWindow="340" windowWidth="27400" windowHeight="16480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -6237,7 +6237,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="381">
+  <cellStyleXfs count="383">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -6619,6 +6619,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -6652,7 +6654,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="381">
+  <cellStyles count="383">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -6847,6 +6849,7 @@
     <cellStyle name="Followed Hyperlink" xfId="376" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="378" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="380" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="382" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -7033,6 +7036,7 @@
     <cellStyle name="Hyperlink" xfId="375" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="377" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="379" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="381" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -9035,7 +9039,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:G42" firstHeaderRow="2" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="8">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -9718,8 +9722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9785,14 +9789,14 @@
         <v>1843</v>
       </c>
       <c r="F5" s="9" t="str">
-        <f>Base_identifier&amp;C5&amp;"."&amp;E5</f>
+        <f t="shared" ref="F5:F36" si="0">Base_identifier&amp;C5&amp;"."&amp;E5</f>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/TIFF.bitsPerSample</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>1831</v>
       </c>
       <c r="H5" s="12" t="str">
-        <f>IF(C5=C4,"","&lt;/table&gt;&lt;h3 id="""&amp;C5&amp;"""&gt;Requirements Class "&amp;C5&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C5&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F5&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G5&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" ref="H5:H36" si="1">IF(C5=C4,"","&lt;/table&gt;&lt;h3 id="""&amp;C5&amp;"""&gt;Requirements Class "&amp;C5&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C5&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F5&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G5&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
         <v>&lt;/table&gt;&lt;h3 id="TIFF"&gt;Requirements Class TIFF&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/TIFF&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/TIFF.bitsPerSample&lt;br/&gt;&lt;i&gt;The BitsPerSample field in the TIFF Image File Directory defines the number of bits per component&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -9812,14 +9816,14 @@
         <v>1840</v>
       </c>
       <c r="F6" s="9" t="str">
-        <f>Base_identifier&amp;C6&amp;"."&amp;E6</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/TIFF.byteOrder</v>
       </c>
       <c r="G6" s="9" t="s">
         <v>22</v>
       </c>
       <c r="H6" s="12" t="str">
-        <f>IF(C6=C5,"","&lt;/table&gt;&lt;h3 id="""&amp;C6&amp;"""&gt;Requirements Class "&amp;C6&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C6&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F6&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G6&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/TIFF.byteOrder&lt;br/&gt;&lt;i&gt;The first two bytes of the GeoTIFF file SHALL be equal to "I" (ASCII) (49 in hexadecimal) for TIFF files encoded using ‘Little-Endian’ and SHALL be equal to "M" (ASCII) (4D in hexadecimal) for TIFF files encoded using ‘Big-Endian’&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -9839,14 +9843,14 @@
         <v>1937</v>
       </c>
       <c r="F7" s="9" t="str">
-        <f>Base_identifier&amp;C7&amp;"."&amp;E7</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/TIFF.DateTime</v>
       </c>
       <c r="G7" s="9" t="s">
         <v>1936</v>
       </c>
       <c r="H7" s="12" t="str">
-        <f>IF(C7=C6,"","&lt;/table&gt;&lt;h3 id="""&amp;C7&amp;"""&gt;Requirements Class "&amp;C7&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C7&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F7&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G7&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/TIFF.DateTime&lt;br/&gt;&lt;i&gt;The format for the field in ASCII type is “YYYY:MM:DD HH:MM:SS” with 24 hour time used for the hours and one space character between the date and time, and one terminating NUL character. The length of the string, including the terminating NUL, is 20 bytes. All dates and times shall be expressed in Coordinated Universal Time (UTC).&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -9866,14 +9870,14 @@
         <v>1846</v>
       </c>
       <c r="F8" s="9" t="str">
-        <f>Base_identifier&amp;C8&amp;"."&amp;E8</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/TIFF.double</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>3</v>
       </c>
       <c r="H8" s="12" t="str">
-        <f>IF(C8=C7,"","&lt;/table&gt;&lt;h3 id="""&amp;C8&amp;"""&gt;Requirements Class "&amp;C8&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C8&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F8&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G8&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/TIFF.double&lt;br/&gt;&lt;i&gt;GeoTIFF requires support for all documented TIFF 6.0 tag data-types, and in particular requires the IEEE double-precision floating point "DOUBLE" type tag.&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -9893,14 +9897,14 @@
         <v>1847</v>
       </c>
       <c r="F9" s="9" t="str">
-        <f>Base_identifier&amp;C9&amp;"."&amp;E9</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/TIFF.fileStructure</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>5</v>
       </c>
       <c r="H9" s="12" t="str">
-        <f>IF(C9=C8,"","&lt;/table&gt;&lt;h3 id="""&amp;C9&amp;"""&gt;Requirements Class "&amp;C9&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C9&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F9&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G9&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/TIFF.fileStructure&lt;br/&gt;&lt;i&gt;A GeoTIFF file is a TIFF 6.0 file, and inherits the file structure as described in the corresponding portion of the TIFF spec.&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -9920,14 +9924,14 @@
         <v>1845</v>
       </c>
       <c r="F10" s="9" t="str">
-        <f>Base_identifier&amp;C10&amp;"."&amp;E10</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/TIFF.griddedValueDataTypes</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>1833</v>
       </c>
       <c r="H10" s="12" t="str">
-        <f>IF(C10=C9,"","&lt;/table&gt;&lt;h3 id="""&amp;C10&amp;"""&gt;Requirements Class "&amp;C10&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C10&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F10&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G10&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/TIFF.griddedValueDataTypes&lt;br/&gt;&lt;i&gt;For gridded data (e.g. elevation data, matrices of lat/lon values, etc.), the range (data) values MAY be stored in additional representations to include 8-bit and 16-bit signed integer and 32-bit floating point.&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -9947,14 +9951,14 @@
         <v>1841</v>
       </c>
       <c r="F11" s="9" t="str">
-        <f>Base_identifier&amp;C11&amp;"."&amp;E11</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/TIFF.IFD</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>1829</v>
       </c>
       <c r="H11" s="12" t="str">
-        <f>IF(C11=C10,"","&lt;/table&gt;&lt;h3 id="""&amp;C11&amp;"""&gt;Requirements Class "&amp;C11&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C11&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F11&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G11&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/TIFF.IFD&lt;br/&gt;&lt;i&gt;There must be at least 1 IFD in a TIFF file and each IFD must have at least one entry.&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -9974,14 +9978,14 @@
         <v>1842</v>
       </c>
       <c r="F12" s="9" t="str">
-        <f>Base_identifier&amp;C12&amp;"."&amp;E12</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/TIFF.IFDCount</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>1830</v>
       </c>
       <c r="H12" s="12" t="str">
-        <f>IF(C12=C11,"","&lt;/table&gt;&lt;h3 id="""&amp;C12&amp;"""&gt;Requirements Class "&amp;C12&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C12&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F12&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G12&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/TIFF.IFDCount&lt;br/&gt;&lt;i&gt;The maximum nuber of IFDs in a GeoTIFF is two, with the second IFD only used to support a transparency mask.&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10001,14 +10005,14 @@
         <v>1844</v>
       </c>
       <c r="F13" s="9" t="str">
-        <f>Base_identifier&amp;C13&amp;"."&amp;E13</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/TIFF.imageryValueDataTypes</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>1834</v>
       </c>
       <c r="H13" s="12" t="str">
-        <f>IF(C13=C12,"","&lt;/table&gt;&lt;h3 id="""&amp;C13&amp;"""&gt;Requirements Class "&amp;C13&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C13&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F13&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G13&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/TIFF.imageryValueDataTypes&lt;br/&gt;&lt;i&gt;For imagery, the range (data) values SHALL be unsigned integer data, 8 or 16-bits-per-band.&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10028,14 +10032,14 @@
         <v>1848</v>
       </c>
       <c r="F14" s="9" t="str">
-        <f>Base_identifier&amp;C14&amp;"."&amp;E14</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/TIFF.noPrivateInformation</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>6</v>
       </c>
       <c r="H14" s="12" t="str">
-        <f>IF(C14=C13,"","&lt;/table&gt;&lt;h3 id="""&amp;C14&amp;"""&gt;Requirements Class "&amp;C14&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C14&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F14&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G14&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/TIFF.noPrivateInformation&lt;br/&gt;&lt;i&gt;All GeoTIFF specific information is encoded in several additional reserved TIFF tags, and contains no private Image File Directories (IFD's), binary structures or other private information invisible to standard TIFF readers&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10055,14 +10059,14 @@
         <v>1849</v>
       </c>
       <c r="F15" s="9" t="str">
-        <f>Base_identifier&amp;C15&amp;"."&amp;E15</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/TIFF.tagOrder</v>
       </c>
       <c r="G15" s="9" t="s">
         <v>16</v>
       </c>
       <c r="H15" s="12" t="str">
-        <f>IF(C15=C14,"","&lt;/table&gt;&lt;h3 id="""&amp;C15&amp;"""&gt;Requirements Class "&amp;C15&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C15&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F15&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G15&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/TIFF.tagOrder&lt;br/&gt;&lt;i&gt;GeoKey entries SHALL be written within the CoordSystemInfoTag in tag-ID sorted order.&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10082,14 +10086,14 @@
         <v>1853</v>
       </c>
       <c r="F16" s="9" t="str">
-        <f>Base_identifier&amp;C16&amp;"."&amp;E16</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyDirectoryTag.count</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>8</v>
       </c>
       <c r="H16" s="12" t="str">
-        <f>IF(C16=C15,"","&lt;/table&gt;&lt;h3 id="""&amp;C16&amp;"""&gt;Requirements Class "&amp;C16&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C16&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F16&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G16&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;/table&gt;&lt;h3 id="GeoKeyDirectoryTag"&gt;Requirements Class GeoKeyDirectoryTag&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyDirectoryTag&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyDirectoryTag.count&lt;br/&gt;&lt;i&gt;The GeoKeyDirectoryTag SHALL include at least 4 keys (short integers) as header information&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10109,14 +10113,14 @@
         <v>1851</v>
       </c>
       <c r="F17" s="9" t="str">
-        <f>Base_identifier&amp;C17&amp;"."&amp;E17</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyDirectoryTag.ID</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>7</v>
       </c>
       <c r="H17" s="12" t="str">
-        <f>IF(C17=C16,"","&lt;/table&gt;&lt;h3 id="""&amp;C17&amp;"""&gt;Requirements Class "&amp;C17&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C17&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F17&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G17&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyDirectoryTag.ID&lt;br/&gt;&lt;i&gt;The GeoKeyDirectoryTag SHALL have ID = 34735&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10136,14 +10140,14 @@
         <v>1854</v>
       </c>
       <c r="F18" s="9" t="str">
-        <f>Base_identifier&amp;C18&amp;"."&amp;E18</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyDirectoryTag.keyDirectoryVersion</v>
       </c>
       <c r="G18" s="9" t="s">
         <v>1939</v>
       </c>
       <c r="H18" s="12" t="str">
-        <f>IF(C18=C17,"","&lt;/table&gt;&lt;h3 id="""&amp;C18&amp;"""&gt;Requirements Class "&amp;C18&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C18&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F18&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G18&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyDirectoryTag.keyDirectoryVersion&lt;br/&gt;&lt;i&gt;The first unsigned short integer in the GeoKeyDirectoryTag SHALL hold the KeyDirectoryVersion.&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10163,14 +10167,14 @@
         <v>1858</v>
       </c>
       <c r="F19" s="9" t="str">
-        <f>Base_identifier&amp;C19&amp;"."&amp;E19</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyDirectoryTag.keyEntrySetCount</v>
       </c>
       <c r="G19" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H19" s="12" t="str">
-        <f>IF(C19=C18,"","&lt;/table&gt;&lt;h3 id="""&amp;C19&amp;"""&gt;Requirements Class "&amp;C19&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C19&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F19&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G19&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyDirectoryTag.keyEntrySetCount&lt;br/&gt;&lt;i&gt;The GeoKeyDirectoryTag SHALL hold NumberOfKeys KeyEntry Sets in addition to the header information&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10190,14 +10194,14 @@
         <v>1855</v>
       </c>
       <c r="F20" s="9" t="str">
-        <f>Base_identifier&amp;C20&amp;"."&amp;E20</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyDirectoryTag.keyRevision</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>1940</v>
       </c>
       <c r="H20" s="12" t="str">
-        <f>IF(C20=C19,"","&lt;/table&gt;&lt;h3 id="""&amp;C20&amp;"""&gt;Requirements Class "&amp;C20&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C20&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F20&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G20&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyDirectoryTag.keyRevision&lt;br/&gt;&lt;i&gt;The second unsigned short integer in the GeoKeyDirectoryTag SHALL hold the KeyRevision.&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10217,14 +10221,14 @@
         <v>1856</v>
       </c>
       <c r="F21" s="9" t="str">
-        <f>Base_identifier&amp;C21&amp;"."&amp;E21</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyDirectoryTag.minorRevision</v>
       </c>
       <c r="G21" s="9" t="s">
         <v>1941</v>
       </c>
       <c r="H21" s="12" t="str">
-        <f>IF(C21=C20,"","&lt;/table&gt;&lt;h3 id="""&amp;C21&amp;"""&gt;Requirements Class "&amp;C21&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C21&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F21&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G21&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyDirectoryTag.minorRevision&lt;br/&gt;&lt;i&gt;The third unsigned short integer in the GeoKeyDirectoryTag SHALL hold the MinorRevision.&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10244,14 +10248,14 @@
         <v>1857</v>
       </c>
       <c r="F22" s="9" t="str">
-        <f>Base_identifier&amp;C22&amp;"."&amp;E22</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyDirectoryTag.numberOfKeys</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>1942</v>
       </c>
       <c r="H22" s="12" t="str">
-        <f>IF(C22=C21,"","&lt;/table&gt;&lt;h3 id="""&amp;C22&amp;"""&gt;Requirements Class "&amp;C22&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C22&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F22&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G22&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyDirectoryTag.numberOfKeys&lt;br/&gt;&lt;i&gt;The fourth unsigned short integer in the GeoKeyDirectoryTag SHALL hold the NumberOfKeys defined in the rest of the GeoKeyDirectoryTag.&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10271,14 +10275,14 @@
         <v>1852</v>
       </c>
       <c r="F23" s="9" t="str">
-        <f>Base_identifier&amp;C23&amp;"."&amp;E23</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyDirectoryTag.type</v>
       </c>
       <c r="G23" s="9" t="s">
         <v>1938</v>
       </c>
       <c r="H23" s="12" t="str">
-        <f>IF(C23=C22,"","&lt;/table&gt;&lt;h3 id="""&amp;C23&amp;"""&gt;Requirements Class "&amp;C23&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C23&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F23&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G23&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyDirectoryTag.type&lt;br/&gt;&lt;i&gt;The GeoKeyDirectoryTag SHALL have type = SHORT (2-byte unsigned integer)&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10298,14 +10302,14 @@
         <v>1887</v>
       </c>
       <c r="F24" s="9" t="str">
-        <f>Base_identifier&amp;C24&amp;"."&amp;E24</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyCode.undefined</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>49</v>
       </c>
       <c r="H24" s="12" t="str">
-        <f>IF(C24=C23,"","&lt;/table&gt;&lt;h3 id="""&amp;C24&amp;"""&gt;Requirements Class "&amp;C24&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C24&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F24&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G24&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;/table&gt;&lt;h3 id="GeoKeyCode"&gt;Requirements Class GeoKeyCode&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyCode&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyCode.undefined&lt;br/&gt;&lt;i&gt;GeoKeys with a value of zero SHALL indicate intentionally omitted parameters&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10325,14 +10329,14 @@
         <v>1888</v>
       </c>
       <c r="F25" s="9" t="str">
-        <f>Base_identifier&amp;C25&amp;"."&amp;E25</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyCode.userDefined</v>
       </c>
       <c r="G25" s="9" t="s">
         <v>50</v>
       </c>
       <c r="H25" s="12" t="str">
-        <f>IF(C25=C24,"","&lt;/table&gt;&lt;h3 id="""&amp;C25&amp;"""&gt;Requirements Class "&amp;C25&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C25&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F25&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G25&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyCode.userDefined&lt;br/&gt;&lt;i&gt;GeoKeys with a value of 32767 SHALL indicate user-defined parameters&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10352,14 +10356,14 @@
         <v>1853</v>
       </c>
       <c r="F26" s="9" t="str">
-        <f>Base_identifier&amp;C26&amp;"."&amp;E26</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeoAsciiParamsTag.count</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>2024</v>
       </c>
       <c r="H26" s="12" t="str">
-        <f>IF(C26=C25,"","&lt;/table&gt;&lt;h3 id="""&amp;C26&amp;"""&gt;Requirements Class "&amp;C26&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C26&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F26&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G26&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;/table&gt;&lt;h3 id="GeoAsciiParamsTag"&gt;Requirements Class GeoAsciiParamsTag&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoAsciiParamsTag&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoAsciiParamsTag.count&lt;br/&gt;&lt;i&gt;The GeoAsciiParamsTag MAY hold any number of key parameters with type = ASCII. (May not be necessary, the same as keyentry.count) &lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10379,14 +10383,14 @@
         <v>1851</v>
       </c>
       <c r="F27" s="9" t="str">
-        <f>Base_identifier&amp;C27&amp;"."&amp;E27</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeoAsciiParamsTag.ID</v>
       </c>
       <c r="G27" s="9" t="s">
         <v>12</v>
       </c>
       <c r="H27" s="12" t="str">
-        <f>IF(C27=C26,"","&lt;/table&gt;&lt;h3 id="""&amp;C27&amp;"""&gt;Requirements Class "&amp;C27&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C27&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F27&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G27&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoAsciiParamsTag.ID&lt;br/&gt;&lt;i&gt;The GeoAsciiParamsTag SHALL have ID = 34737&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10406,14 +10410,14 @@
         <v>1868</v>
       </c>
       <c r="F28" s="9" t="str">
-        <f>Base_identifier&amp;C28&amp;"."&amp;E28</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeoAsciiParamsTag.NULLRead</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>15</v>
       </c>
       <c r="H28" s="12" t="str">
-        <f>IF(C28=C27,"","&lt;/table&gt;&lt;h3 id="""&amp;C28&amp;"""&gt;Requirements Class "&amp;C28&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C28&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F28&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G28&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoAsciiParamsTag.NULLRead&lt;br/&gt;&lt;i&gt;Pipe characters (“|”) in the GeoAsciiParamsTag SHALL be converted NULL characters before returning strings to the client&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10433,14 +10437,14 @@
         <v>1867</v>
       </c>
       <c r="F29" s="9" t="str">
-        <f>Base_identifier&amp;C29&amp;"."&amp;E29</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeoAsciiParamsTag.NULLWrite</v>
       </c>
       <c r="G29" s="9" t="s">
         <v>14</v>
       </c>
       <c r="H29" s="12" t="str">
-        <f>IF(C29=C28,"","&lt;/table&gt;&lt;h3 id="""&amp;C29&amp;"""&gt;Requirements Class "&amp;C29&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C29&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F29&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G29&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoAsciiParamsTag.NULLWrite&lt;br/&gt;&lt;i&gt;NULL characters used to terminate strings in the GeoAsciiParamsTag SHALL be converted to a “|” (pipe) prior to being written into the GeoAsciiParamsTag&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10460,14 +10464,14 @@
         <v>1852</v>
       </c>
       <c r="F30" s="9" t="str">
-        <f>Base_identifier&amp;C30&amp;"."&amp;E30</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeoAsciiParamsTag.type</v>
       </c>
       <c r="G30" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H30" s="12" t="str">
-        <f>IF(C30=C29,"","&lt;/table&gt;&lt;h3 id="""&amp;C30&amp;"""&gt;Requirements Class "&amp;C30&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C30&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F30&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G30&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoAsciiParamsTag.type&lt;br/&gt;&lt;i&gt;The GeoAsciiParamsTag SHALL have type = ASCII&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10488,14 +10492,14 @@
         <v>1891</v>
       </c>
       <c r="F31" s="9" t="str">
-        <f>Base_identifier&amp;C31&amp;"."&amp;E31</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GTModelTypeGeoKey.geocentric</v>
       </c>
       <c r="G31" s="9" t="s">
         <v>2026</v>
       </c>
       <c r="H31" s="12" t="str">
-        <f>IF(C31=C30,"","&lt;/table&gt;&lt;h3 id="""&amp;C31&amp;"""&gt;Requirements Class "&amp;C31&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C31&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F31&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G31&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;/table&gt;&lt;h3 id="GTModelTypeGeoKey"&gt;Requirements Class GTModelTypeGeoKey&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GTModelTypeGeoKey&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GTModelTypeGeoKey.geocentric&lt;br/&gt;&lt;i&gt;A value of 3 for the GTModelTypeGeoKey SHALL indicate a geocentric(X,Y,Z) coordinate system &lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10516,14 +10520,14 @@
         <v>1884</v>
       </c>
       <c r="F32" s="9" t="str">
-        <f>Base_identifier&amp;C32&amp;"."&amp;E32</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GTModelTypeGeoKey.geographic</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>55</v>
       </c>
       <c r="H32" s="12" t="str">
-        <f>IF(C32=C31,"","&lt;/table&gt;&lt;h3 id="""&amp;C32&amp;"""&gt;Requirements Class "&amp;C32&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C32&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F32&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G32&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GTModelTypeGeoKey.geographic&lt;br/&gt;&lt;i&gt;A value of 2 for the GTModelTypeGeoKey SHALL indicate a geographic latitude-longitude  coordinate system &lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10544,14 +10548,14 @@
         <v>1851</v>
       </c>
       <c r="F33" s="9" t="str">
-        <f>Base_identifier&amp;C33&amp;"."&amp;E33</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GTModelTypeGeoKey.ID</v>
       </c>
       <c r="G33" s="9" t="s">
         <v>52</v>
       </c>
       <c r="H33" s="12" t="str">
-        <f>IF(C33=C32,"","&lt;/table&gt;&lt;h3 id="""&amp;C33&amp;"""&gt;Requirements Class "&amp;C33&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C33&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F33&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G33&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GTModelTypeGeoKey.ID&lt;br/&gt;&lt;i&gt;The GTModelTypeGeoKey SHALL have ID = 1024&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10572,14 +10576,14 @@
         <v>1890</v>
       </c>
       <c r="F34" s="9" t="str">
-        <f>Base_identifier&amp;C34&amp;"."&amp;E34</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GTModelTypeGeoKey.private</v>
       </c>
       <c r="G34" s="9" t="s">
         <v>60</v>
       </c>
       <c r="H34" s="12" t="str">
-        <f>IF(C34=C33,"","&lt;/table&gt;&lt;h3 id="""&amp;C34&amp;"""&gt;Requirements Class "&amp;C34&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C34&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F34&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G34&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GTModelTypeGeoKey.private&lt;br/&gt;&lt;i&gt;GTModelTypeGeoKey values in the range 32768-65535 SHALL be private&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10600,14 +10604,14 @@
         <v>1885</v>
       </c>
       <c r="F35" s="9" t="str">
-        <f>Base_identifier&amp;C35&amp;"."&amp;E35</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GTModelTypeGeoKey.projected</v>
       </c>
       <c r="G35" s="9" t="s">
         <v>54</v>
       </c>
       <c r="H35" s="12" t="str">
-        <f>IF(C35=C34,"","&lt;/table&gt;&lt;h3 id="""&amp;C35&amp;"""&gt;Requirements Class "&amp;C35&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C35&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F35&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G35&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GTModelTypeGeoKey.projected&lt;br/&gt;&lt;i&gt;A value of 1 for the GTModelTypeGeoKey SHALL indicate a projected coordinate system &lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10628,14 +10632,14 @@
         <v>1882</v>
       </c>
       <c r="F36" s="9" t="str">
-        <f>Base_identifier&amp;C36&amp;"."&amp;E36</f>
+        <f t="shared" si="0"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GTModelTypeGeoKey.reserved</v>
       </c>
       <c r="G36" s="9" t="s">
         <v>59</v>
       </c>
       <c r="H36" s="12" t="str">
-        <f>IF(C36=C35,"","&lt;/table&gt;&lt;h3 id="""&amp;C36&amp;"""&gt;Requirements Class "&amp;C36&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C36&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F36&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G36&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="1"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GTModelTypeGeoKey.reserved&lt;br/&gt;&lt;i&gt;GTModelTypeGeoKey values in the range 1-32766 SHALL be reserved&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10656,14 +10660,14 @@
         <v>1852</v>
       </c>
       <c r="F37" s="9" t="str">
-        <f>Base_identifier&amp;C37&amp;"."&amp;E37</f>
+        <f t="shared" ref="F37:F68" si="2">Base_identifier&amp;C37&amp;"."&amp;E37</f>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GTModelTypeGeoKey.type</v>
       </c>
       <c r="G37" s="9" t="s">
         <v>53</v>
       </c>
       <c r="H37" s="12" t="str">
-        <f>IF(C37=C36,"","&lt;/table&gt;&lt;h3 id="""&amp;C37&amp;"""&gt;Requirements Class "&amp;C37&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C37&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F37&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G37&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" ref="H37:H68" si="3">IF(C37=C36,"","&lt;/table&gt;&lt;h3 id="""&amp;C37&amp;"""&gt;Requirements Class "&amp;C37&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C37&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F37&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G37&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GTModelTypeGeoKey.type&lt;br/&gt;&lt;i&gt;The GTModelTypeGeoKey SHALL have type = SHORT&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10684,14 +10688,14 @@
         <v>1851</v>
       </c>
       <c r="F38" s="9" t="str">
-        <f>Base_identifier&amp;C38&amp;"."&amp;E38</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GTRasterTypeGeoKey.ID</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>57</v>
       </c>
       <c r="H38" s="12" t="str">
-        <f>IF(C38=C37,"","&lt;/table&gt;&lt;h3 id="""&amp;C38&amp;"""&gt;Requirements Class "&amp;C38&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C38&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F38&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G38&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;/table&gt;&lt;h3 id="GTRasterTypeGeoKey"&gt;Requirements Class GTRasterTypeGeoKey&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GTRasterTypeGeoKey&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GTRasterTypeGeoKey.ID&lt;br/&gt;&lt;i&gt;The GTModelTypeGeoKey SHALL have ID = 1025&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10712,14 +10716,14 @@
         <v>1890</v>
       </c>
       <c r="F39" s="9" t="str">
-        <f>Base_identifier&amp;C39&amp;"."&amp;E39</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GTRasterTypeGeoKey.private</v>
       </c>
       <c r="G39" s="9" t="s">
         <v>62</v>
       </c>
       <c r="H39" s="12" t="str">
-        <f>IF(C39=C38,"","&lt;/table&gt;&lt;h3 id="""&amp;C39&amp;"""&gt;Requirements Class "&amp;C39&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C39&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F39&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G39&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GTRasterTypeGeoKey.private&lt;br/&gt;&lt;i&gt;GTRasterTypeGeoKey values in the range 32768-65535 SHALL be private&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10740,14 +10744,14 @@
         <v>1893</v>
       </c>
       <c r="F40" s="9" t="str">
-        <f>Base_identifier&amp;C40&amp;"."&amp;E40</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GTRasterTypeGeoKey.rasterPixelIsArea</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>2027</v>
       </c>
       <c r="H40" s="12" t="str">
-        <f>IF(C40=C39,"","&lt;/table&gt;&lt;h3 id="""&amp;C40&amp;"""&gt;Requirements Class "&amp;C40&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C40&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F40&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G40&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GTRasterTypeGeoKey.rasterPixelIsArea&lt;br/&gt;&lt;i&gt;A value of 1 for the GTRasterTypeGeoKey SHALL indicate that  this raster pixel is an area (for DGIWG profile, this is used by imagery products).&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10768,14 +10772,14 @@
         <v>1894</v>
       </c>
       <c r="F41" s="9" t="str">
-        <f>Base_identifier&amp;C41&amp;"."&amp;E41</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GTRasterTypeGeoKey.rasterPixelIsPoint</v>
       </c>
       <c r="G41" s="9" t="s">
         <v>2028</v>
       </c>
       <c r="H41" s="12" t="str">
-        <f>IF(C41=C40,"","&lt;/table&gt;&lt;h3 id="""&amp;C41&amp;"""&gt;Requirements Class "&amp;C41&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C41&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F41&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G41&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GTRasterTypeGeoKey.rasterPixelIsPoint&lt;br/&gt;&lt;i&gt;A value of 2 for the GTRasterTypeGeoKey SHALL indicate that this raster pixel is a point (for DGIWG profile, this is used for discrete coverage data including elevation data ).&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10796,14 +10800,14 @@
         <v>1882</v>
       </c>
       <c r="F42" s="9" t="str">
-        <f>Base_identifier&amp;C42&amp;"."&amp;E42</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GTRasterTypeGeoKey.reserved</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>61</v>
       </c>
       <c r="H42" s="12" t="str">
-        <f>IF(C42=C41,"","&lt;/table&gt;&lt;h3 id="""&amp;C42&amp;"""&gt;Requirements Class "&amp;C42&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C42&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F42&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G42&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GTRasterTypeGeoKey.reserved&lt;br/&gt;&lt;i&gt;GTRasterTypeGeoKey values in the range 1-32766 SHALL be reserved&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10824,14 +10828,14 @@
         <v>1852</v>
       </c>
       <c r="F43" s="9" t="str">
-        <f>Base_identifier&amp;C43&amp;"."&amp;E43</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GTRasterTypeGeoKey.type</v>
       </c>
       <c r="G43" s="9" t="s">
         <v>53</v>
       </c>
       <c r="H43" s="12" t="str">
-        <f>IF(C43=C42,"","&lt;/table&gt;&lt;h3 id="""&amp;C43&amp;"""&gt;Requirements Class "&amp;C43&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C43&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F43&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G43&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GTRasterTypeGeoKey.type&lt;br/&gt;&lt;i&gt;The GTModelTypeGeoKey SHALL have type = SHORT&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10852,14 +10856,14 @@
         <v>1851</v>
       </c>
       <c r="F44" s="9" t="str">
-        <f>Base_identifier&amp;C44&amp;"."&amp;E44</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GTCitationGeoKey.ID</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>63</v>
       </c>
       <c r="H44" s="12" t="str">
-        <f>IF(C44=C43,"","&lt;/table&gt;&lt;h3 id="""&amp;C44&amp;"""&gt;Requirements Class "&amp;C44&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C44&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F44&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G44&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;/table&gt;&lt;h3 id="GTCitationGeoKey"&gt;Requirements Class GTCitationGeoKey&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GTCitationGeoKey&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GTCitationGeoKey.ID&lt;br/&gt;&lt;i&gt;The GTCitationGeoKey SHALL have ID = 1026&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10880,14 +10884,14 @@
         <v>1852</v>
       </c>
       <c r="F45" s="9" t="str">
-        <f>Base_identifier&amp;C45&amp;"."&amp;E45</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GTCitationGeoKey.type</v>
       </c>
       <c r="G45" s="9" t="s">
         <v>64</v>
       </c>
       <c r="H45" s="12" t="str">
-        <f>IF(C45=C44,"","&lt;/table&gt;&lt;h3 id="""&amp;C45&amp;"""&gt;Requirements Class "&amp;C45&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C45&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F45&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G45&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GTCitationGeoKey.type&lt;br/&gt;&lt;i&gt;The GTCitationGeoKey SHALL have type = ASCII&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10908,14 +10912,14 @@
         <v>1951</v>
       </c>
       <c r="F46" s="9" t="str">
-        <f>Base_identifier&amp;C46&amp;"."&amp;E46</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeographicTypeGeoKey.DGIWGReference</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>1950</v>
       </c>
       <c r="H46" s="12" t="str">
-        <f>IF(C46=C45,"","&lt;/table&gt;&lt;h3 id="""&amp;C46&amp;"""&gt;Requirements Class "&amp;C46&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C46&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F46&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G46&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;/table&gt;&lt;h3 id="GeographicTypeGeoKey"&gt;Requirements Class GeographicTypeGeoKey&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeographicTypeGeoKey&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeographicTypeGeoKey.DGIWGReference&lt;br/&gt;&lt;i&gt;WGS84 + may include Reference document citation (EPSG, DGIWG Registry or [DMA TR 8350.2])&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10936,14 +10940,14 @@
         <v>1949</v>
       </c>
       <c r="F47" s="9" t="str">
-        <f>Base_identifier&amp;C47&amp;"."&amp;E47</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeographicTypeGeoKey.DGIWGValues</v>
       </c>
       <c r="G47" s="9" t="s">
         <v>1952</v>
       </c>
       <c r="H47" s="12" t="str">
-        <f>IF(C47=C46,"","&lt;/table&gt;&lt;h3 id="""&amp;C47&amp;"""&gt;Requirements Class "&amp;C47&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C47&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F47&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G47&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeographicTypeGeoKey.DGIWGValues&lt;br/&gt;&lt;i&gt;SHALL be 4326 (GCS_WGS84) or 4030 (GCSE_WGS84, not recommended by GeoTIFF)&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10964,14 +10968,14 @@
         <v>1899</v>
       </c>
       <c r="F48" s="9" t="str">
-        <f>Base_identifier&amp;C48&amp;"."&amp;E48</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeographicTypeGeoKey.EPSGDatum</v>
       </c>
       <c r="G48" s="9" t="s">
         <v>70</v>
       </c>
       <c r="H48" s="12" t="str">
-        <f>IF(C48=C47,"","&lt;/table&gt;&lt;h3 id="""&amp;C48&amp;"""&gt;Requirements Class "&amp;C48&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C48&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F48&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G48&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeographicTypeGeoKey.EPSGDatum&lt;br/&gt;&lt;i&gt;GeographicTypeGeoKey values in the range 4200-4999 SHALL be EPSG GCS Based on EPSG Datum&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -10992,14 +10996,14 @@
         <v>1898</v>
       </c>
       <c r="F49" s="9" t="str">
-        <f>Base_identifier&amp;C49&amp;"."&amp;E49</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeographicTypeGeoKey.EPSGEllipsoid</v>
       </c>
       <c r="G49" s="9" t="s">
         <v>69</v>
       </c>
       <c r="H49" s="12" t="str">
-        <f>IF(C49=C48,"","&lt;/table&gt;&lt;h3 id="""&amp;C49&amp;"""&gt;Requirements Class "&amp;C49&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C49&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F49&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G49&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeographicTypeGeoKey.EPSGEllipsoid&lt;br/&gt;&lt;i&gt;GeographicTypeGeoKey values in the range 4000-4199 SHALL be EPSG GCS Based on Ellipsoid only&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11020,14 +11024,14 @@
         <v>1851</v>
       </c>
       <c r="F50" s="9" t="str">
-        <f>Base_identifier&amp;C50&amp;"."&amp;E50</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeographicTypeGeoKey.ID</v>
       </c>
       <c r="G50" s="9" t="s">
         <v>66</v>
       </c>
       <c r="H50" s="12" t="str">
-        <f>IF(C50=C49,"","&lt;/table&gt;&lt;h3 id="""&amp;C50&amp;"""&gt;Requirements Class "&amp;C50&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C50&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F50&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G50&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeographicTypeGeoKey.ID&lt;br/&gt;&lt;i&gt;The GeographicTypeGeoKey SHALL have ID = 2048&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11048,14 +11052,14 @@
         <v>1897</v>
       </c>
       <c r="F51" s="9" t="str">
-        <f>Base_identifier&amp;C51&amp;"."&amp;E51</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeographicTypeGeoKey.obsolete</v>
       </c>
       <c r="G51" s="9" t="s">
         <v>75</v>
       </c>
       <c r="H51" s="12" t="str">
-        <f>IF(C51=C50,"","&lt;/table&gt;&lt;h3 id="""&amp;C51&amp;"""&gt;Requirements Class "&amp;C51&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C51&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F51&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G51&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeographicTypeGeoKey.obsolete&lt;br/&gt;&lt;i&gt;GeographicTypeGeoKey values in the range 1-1000 SHALL be obsolete EPSG/POSC Geographic Codes&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11076,14 +11080,14 @@
         <v>1890</v>
       </c>
       <c r="F52" s="9" t="str">
-        <f>Base_identifier&amp;C52&amp;"."&amp;E52</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeographicTypeGeoKey.private</v>
       </c>
       <c r="G52" s="9" t="s">
         <v>68</v>
       </c>
       <c r="H52" s="12" t="str">
-        <f>IF(C52=C51,"","&lt;/table&gt;&lt;h3 id="""&amp;C52&amp;"""&gt;Requirements Class "&amp;C52&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C52&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F52&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G52&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeographicTypeGeoKey.private&lt;br/&gt;&lt;i&gt;GeographicTypeGeoKey values in the range 32768-65535 SHALL be private&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11104,14 +11108,14 @@
         <v>1882</v>
       </c>
       <c r="F53" s="9" t="str">
-        <f>Base_identifier&amp;C53&amp;"."&amp;E53</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeographicTypeGeoKey.reserved</v>
       </c>
       <c r="G53" s="9" t="s">
         <v>77</v>
       </c>
       <c r="H53" s="12" t="str">
-        <f>IF(C53=C52,"","&lt;/table&gt;&lt;h3 id="""&amp;C53&amp;"""&gt;Requirements Class "&amp;C53&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C53&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F53&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G53&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeographicTypeGeoKey.reserved&lt;br/&gt;&lt;i&gt;GeographicTypeGeoKey values in the range 1001-3999 and 5000-32766 SHALL be reserved&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11132,14 +11136,14 @@
         <v>1852</v>
       </c>
       <c r="F54" s="9" t="str">
-        <f>Base_identifier&amp;C54&amp;"."&amp;E54</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeographicTypeGeoKey.type</v>
       </c>
       <c r="G54" s="9" t="s">
         <v>65</v>
       </c>
       <c r="H54" s="12" t="str">
-        <f>IF(C54=C53,"","&lt;/table&gt;&lt;h3 id="""&amp;C54&amp;"""&gt;Requirements Class "&amp;C54&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C54&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F54&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G54&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeographicTypeGeoKey.type&lt;br/&gt;&lt;i&gt;The GeographicTypeGeoKey SHALL have type = SHORT&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11160,14 +11164,14 @@
         <v>1851</v>
       </c>
       <c r="F55" s="9" t="str">
-        <f>Base_identifier&amp;C55&amp;"."&amp;E55</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogCitationGeoKey.ID</v>
       </c>
       <c r="G55" s="9" t="s">
         <v>72</v>
       </c>
       <c r="H55" s="12" t="str">
-        <f>IF(C55=C54,"","&lt;/table&gt;&lt;h3 id="""&amp;C55&amp;"""&gt;Requirements Class "&amp;C55&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C55&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F55&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G55&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;/table&gt;&lt;h3 id="GeogCitationGeoKey"&gt;Requirements Class GeogCitationGeoKey&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogCitationGeoKey&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogCitationGeoKey.ID&lt;br/&gt;&lt;i&gt;The GeogCitationGeoKey SHALL have ID = 2049&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11188,14 +11192,14 @@
         <v>1852</v>
       </c>
       <c r="F56" s="9" t="str">
-        <f>Base_identifier&amp;C56&amp;"."&amp;E56</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogCitationGeoKey.type</v>
       </c>
       <c r="G56" s="9" t="s">
         <v>71</v>
       </c>
       <c r="H56" s="12" t="str">
-        <f>IF(C56=C55,"","&lt;/table&gt;&lt;h3 id="""&amp;C56&amp;"""&gt;Requirements Class "&amp;C56&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C56&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F56&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G56&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogCitationGeoKey.type&lt;br/&gt;&lt;i&gt;The GeogCitationGeoKey SHALL have type = ASCII&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11216,14 +11220,14 @@
         <v>1851</v>
       </c>
       <c r="F57" s="9" t="str">
-        <f>Base_identifier&amp;C57&amp;"."&amp;E57</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogGeodeticDatumGeoKey.ID</v>
       </c>
       <c r="G57" s="9" t="s">
         <v>73</v>
       </c>
       <c r="H57" s="12" t="str">
-        <f>IF(C57=C56,"","&lt;/table&gt;&lt;h3 id="""&amp;C57&amp;"""&gt;Requirements Class "&amp;C57&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C57&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F57&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G57&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;/table&gt;&lt;h3 id="GeogGeodeticDatumGeoKey"&gt;Requirements Class GeogGeodeticDatumGeoKey&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogGeodeticDatumGeoKey&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogGeodeticDatumGeoKey.ID&lt;br/&gt;&lt;i&gt;The GeogCitationGeoKey SHALL have ID = 2050&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11244,14 +11248,14 @@
         <v>1852</v>
       </c>
       <c r="F58" s="9" t="str">
-        <f>Base_identifier&amp;C58&amp;"."&amp;E58</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogGeodeticDatumGeoKey.type</v>
       </c>
       <c r="G58" s="9" t="s">
         <v>74</v>
       </c>
       <c r="H58" s="12" t="str">
-        <f>IF(C58=C57,"","&lt;/table&gt;&lt;h3 id="""&amp;C58&amp;"""&gt;Requirements Class "&amp;C58&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C58&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F58&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G58&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogGeodeticDatumGeoKey.type&lt;br/&gt;&lt;i&gt;The GeogCitationGeoKey SHALL have type = SHORT&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11272,14 +11276,14 @@
         <v>1898</v>
       </c>
       <c r="F59" s="9" t="str">
-        <f>Base_identifier&amp;C59&amp;"."&amp;E59</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogPrimeMeridianGeoKey.EPSGEllipsoid</v>
       </c>
       <c r="G59" s="9" t="s">
         <v>90</v>
       </c>
       <c r="H59" s="12" t="str">
-        <f>IF(C59=C58,"","&lt;/table&gt;&lt;h3 id="""&amp;C59&amp;"""&gt;Requirements Class "&amp;C59&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C59&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F59&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G59&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;/table&gt;&lt;h3 id="GeogPrimeMeridianGeoKey"&gt;Requirements Class GeogPrimeMeridianGeoKey&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogPrimeMeridianGeoKey&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogPrimeMeridianGeoKey.EPSGEllipsoid&lt;br/&gt;&lt;i&gt;GeogPrimeMeridianGeoKey  values in the range 8000-8999 SHALL be EPSG Prime Meridian Codes&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11300,14 +11304,14 @@
         <v>1851</v>
       </c>
       <c r="F60" s="9" t="str">
-        <f>Base_identifier&amp;C60&amp;"."&amp;E60</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogPrimeMeridianGeoKey.ID</v>
       </c>
       <c r="G60" s="9" t="s">
         <v>85</v>
       </c>
       <c r="H60" s="12" t="str">
-        <f>IF(C60=C59,"","&lt;/table&gt;&lt;h3 id="""&amp;C60&amp;"""&gt;Requirements Class "&amp;C60&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C60&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F60&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G60&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogPrimeMeridianGeoKey.ID&lt;br/&gt;&lt;i&gt;The GeogPrimeMeridianGeoKey SHALL have ID = 2051&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11328,14 +11332,14 @@
         <v>1897</v>
       </c>
       <c r="F61" s="9" t="str">
-        <f>Base_identifier&amp;C61&amp;"."&amp;E61</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogPrimeMeridianGeoKey.obsolete</v>
       </c>
       <c r="G61" s="9" t="s">
         <v>88</v>
       </c>
       <c r="H61" s="12" t="str">
-        <f>IF(C61=C60,"","&lt;/table&gt;&lt;h3 id="""&amp;C61&amp;"""&gt;Requirements Class "&amp;C61&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C61&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F61&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G61&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogPrimeMeridianGeoKey.obsolete&lt;br/&gt;&lt;i&gt;GeogPrimeMeridianGeoKey  values in the range 1-100 SHALL be obsolete EPSG/POSC Datum Codes&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11356,14 +11360,14 @@
         <v>1890</v>
       </c>
       <c r="F62" s="9" t="str">
-        <f>Base_identifier&amp;C62&amp;"."&amp;E62</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogPrimeMeridianGeoKey.private</v>
       </c>
       <c r="G62" s="9" t="s">
         <v>87</v>
       </c>
       <c r="H62" s="12" t="str">
-        <f>IF(C62=C61,"","&lt;/table&gt;&lt;h3 id="""&amp;C62&amp;"""&gt;Requirements Class "&amp;C62&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C62&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F62&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G62&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogPrimeMeridianGeoKey.private&lt;br/&gt;&lt;i&gt;GeogPrimeMeridianGeoKey  values in the range 32768-65535 SHALL be private&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11384,14 +11388,14 @@
         <v>1882</v>
       </c>
       <c r="F63" s="9" t="str">
-        <f>Base_identifier&amp;C63&amp;"."&amp;E63</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogPrimeMeridianGeoKey.reserved</v>
       </c>
       <c r="G63" s="9" t="s">
         <v>89</v>
       </c>
       <c r="H63" s="12" t="str">
-        <f>IF(C63=C62,"","&lt;/table&gt;&lt;h3 id="""&amp;C63&amp;"""&gt;Requirements Class "&amp;C63&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C63&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F63&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G63&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogPrimeMeridianGeoKey.reserved&lt;br/&gt;&lt;i&gt;GeogPrimeMeridianGeoKey  values in the range 101-7999 and 9000-32766 SHALL be reserved&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11412,14 +11416,14 @@
         <v>1852</v>
       </c>
       <c r="F64" s="9" t="str">
-        <f>Base_identifier&amp;C64&amp;"."&amp;E64</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogPrimeMeridianGeoKey.type</v>
       </c>
       <c r="G64" s="9" t="s">
         <v>86</v>
       </c>
       <c r="H64" s="12" t="str">
-        <f>IF(C64=C63,"","&lt;/table&gt;&lt;h3 id="""&amp;C64&amp;"""&gt;Requirements Class "&amp;C64&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C64&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F64&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G64&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogPrimeMeridianGeoKey.type&lt;br/&gt;&lt;i&gt;The GeogPrimeMeridianGeoKey SHALL have type = SHORT&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11440,14 +11444,14 @@
         <v>1851</v>
       </c>
       <c r="F65" s="9" t="str">
-        <f>Base_identifier&amp;C65&amp;"."&amp;E65</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogPrimeMeridianLongGeoKey.ID</v>
       </c>
       <c r="G65" s="9" t="s">
         <v>92</v>
       </c>
       <c r="H65" s="12" t="str">
-        <f>IF(C65=C64,"","&lt;/table&gt;&lt;h3 id="""&amp;C65&amp;"""&gt;Requirements Class "&amp;C65&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C65&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F65&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G65&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;/table&gt;&lt;h3 id="GeogPrimeMeridianLongGeoKey"&gt;Requirements Class GeogPrimeMeridianLongGeoKey&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogPrimeMeridianLongGeoKey&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogPrimeMeridianLongGeoKey.ID&lt;br/&gt;&lt;i&gt;The GeogPrimeMeridianLongGeoKey SHALL have ID = 2061&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11468,14 +11472,14 @@
         <v>1852</v>
       </c>
       <c r="F66" s="9" t="str">
-        <f>Base_identifier&amp;C66&amp;"."&amp;E66</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogPrimeMeridianLongGeoKey.type</v>
       </c>
       <c r="G66" s="9" t="s">
         <v>93</v>
       </c>
       <c r="H66" s="12" t="str">
-        <f>IF(C66=C65,"","&lt;/table&gt;&lt;h3 id="""&amp;C66&amp;"""&gt;Requirements Class "&amp;C66&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C66&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F66&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G66&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogPrimeMeridianLongGeoKey.type&lt;br/&gt;&lt;i&gt;The GeogPrimeMeridianLongGeoKey SHALL have type = DOUBLE&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11496,14 +11500,14 @@
         <v>1907</v>
       </c>
       <c r="F67" s="9" t="str">
-        <f>Base_identifier&amp;C67&amp;"."&amp;E67</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogPrimeMeridianLongGeoKey.units</v>
       </c>
       <c r="G67" s="9" t="s">
         <v>94</v>
       </c>
       <c r="H67" s="12" t="str">
-        <f>IF(C67=C66,"","&lt;/table&gt;&lt;h3 id="""&amp;C67&amp;"""&gt;Requirements Class "&amp;C67&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C67&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F67&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G67&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogPrimeMeridianLongGeoKey.units&lt;br/&gt;&lt;i&gt;The GeogPrimeMeridianLongGeoKey SHALL have units = GeogAngularUnits&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11524,14 +11528,14 @@
         <v>1910</v>
       </c>
       <c r="F68" s="9" t="str">
-        <f>Base_identifier&amp;C68&amp;"."&amp;E68</f>
+        <f t="shared" si="2"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogLinearUnitsGeoKey.angular</v>
       </c>
       <c r="G68" s="9" t="s">
         <v>103</v>
       </c>
       <c r="H68" s="12" t="str">
-        <f>IF(C68=C67,"","&lt;/table&gt;&lt;h3 id="""&amp;C68&amp;"""&gt;Requirements Class "&amp;C68&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C68&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F68&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G68&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="3"/>
         <v>&lt;/table&gt;&lt;h3 id="GeogLinearUnitsGeoKey"&gt;Requirements Class GeogLinearUnitsGeoKey&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogLinearUnitsGeoKey&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogLinearUnitsGeoKey.angular&lt;br/&gt;&lt;i&gt;GeogLinearUnitsGeoKey values in the range 9100-9199 SHALL be EPSG angular units&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11552,14 +11556,14 @@
         <v>1851</v>
       </c>
       <c r="F69" s="9" t="str">
-        <f>Base_identifier&amp;C69&amp;"."&amp;E69</f>
+        <f t="shared" ref="F69:F100" si="4">Base_identifier&amp;C69&amp;"."&amp;E69</f>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogLinearUnitsGeoKey.ID</v>
       </c>
       <c r="G69" s="9" t="s">
         <v>98</v>
       </c>
       <c r="H69" s="12" t="str">
-        <f>IF(C69=C68,"","&lt;/table&gt;&lt;h3 id="""&amp;C69&amp;"""&gt;Requirements Class "&amp;C69&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C69&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F69&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G69&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" ref="H69:H100" si="5">IF(C69=C68,"","&lt;/table&gt;&lt;h3 id="""&amp;C69&amp;"""&gt;Requirements Class "&amp;C69&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C69&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F69&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G69&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogLinearUnitsGeoKey.ID&lt;br/&gt;&lt;i&gt;The GeogLinearUnitsGeoKey SHALL have ID = 2052&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11580,14 +11584,14 @@
         <v>1909</v>
       </c>
       <c r="F70" s="9" t="str">
-        <f>Base_identifier&amp;C70&amp;"."&amp;E70</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogLinearUnitsGeoKey.linear</v>
       </c>
       <c r="G70" s="9" t="s">
         <v>102</v>
       </c>
       <c r="H70" s="12" t="str">
-        <f>IF(C70=C69,"","&lt;/table&gt;&lt;h3 id="""&amp;C70&amp;"""&gt;Requirements Class "&amp;C70&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C70&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F70&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G70&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogLinearUnitsGeoKey.linear&lt;br/&gt;&lt;i&gt;GeogLinearUnitsGeoKey values in the range 9000-9099 SHALL be EPSG linear units&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11608,14 +11612,14 @@
         <v>1897</v>
       </c>
       <c r="F71" s="9" t="str">
-        <f>Base_identifier&amp;C71&amp;"."&amp;E71</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogLinearUnitsGeoKey.obsolete</v>
       </c>
       <c r="G71" s="9" t="s">
         <v>100</v>
       </c>
       <c r="H71" s="12" t="str">
-        <f>IF(C71=C70,"","&lt;/table&gt;&lt;h3 id="""&amp;C71&amp;"""&gt;Requirements Class "&amp;C71&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C71&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F71&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G71&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogLinearUnitsGeoKey.obsolete&lt;br/&gt;&lt;i&gt;GeogLinearUnitsGeoKey values in the range 1-2000 SHALL be obsolete GeoTIFF Codes&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11636,14 +11640,14 @@
         <v>1890</v>
       </c>
       <c r="F72" s="9" t="str">
-        <f>Base_identifier&amp;C72&amp;"."&amp;E72</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogLinearUnitsGeoKey.private</v>
       </c>
       <c r="G72" s="9" t="s">
         <v>104</v>
       </c>
       <c r="H72" s="12" t="str">
-        <f>IF(C72=C71,"","&lt;/table&gt;&lt;h3 id="""&amp;C72&amp;"""&gt;Requirements Class "&amp;C72&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C72&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F72&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G72&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogLinearUnitsGeoKey.private&lt;br/&gt;&lt;i&gt;GeogLinearUnitsGeoKey values in the range 32768-65535 SHALL be private&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11664,14 +11668,14 @@
         <v>1882</v>
       </c>
       <c r="F73" s="9" t="str">
-        <f>Base_identifier&amp;C73&amp;"."&amp;E73</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogLinearUnitsGeoKey.reserved</v>
       </c>
       <c r="G73" s="9" t="s">
         <v>101</v>
       </c>
       <c r="H73" s="12" t="str">
-        <f>IF(C73=C72,"","&lt;/table&gt;&lt;h3 id="""&amp;C73&amp;"""&gt;Requirements Class "&amp;C73&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C73&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F73&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G73&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogLinearUnitsGeoKey.reserved&lt;br/&gt;&lt;i&gt;GeogLinearUnitsGeoKey values in the range 2001-8999 SHALL be reserved&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11692,14 +11696,14 @@
         <v>1852</v>
       </c>
       <c r="F74" s="9" t="str">
-        <f>Base_identifier&amp;C74&amp;"."&amp;E74</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogLinearUnitsGeoKey.type</v>
       </c>
       <c r="G74" s="9" t="s">
         <v>99</v>
       </c>
       <c r="H74" s="12" t="str">
-        <f>IF(C74=C73,"","&lt;/table&gt;&lt;h3 id="""&amp;C74&amp;"""&gt;Requirements Class "&amp;C74&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C74&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F74&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G74&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogLinearUnitsGeoKey.type&lt;br/&gt;&lt;i&gt;The GeogLinearUnitsGeoKey SHALL have type = DOUBLE&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11720,14 +11724,14 @@
         <v>1851</v>
       </c>
       <c r="F75" s="9" t="str">
-        <f>Base_identifier&amp;C75&amp;"."&amp;E75</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogLinearUnitSizeGeoKey.ID</v>
       </c>
       <c r="G75" s="9" t="s">
         <v>105</v>
       </c>
       <c r="H75" s="12" t="str">
-        <f>IF(C75=C74,"","&lt;/table&gt;&lt;h3 id="""&amp;C75&amp;"""&gt;Requirements Class "&amp;C75&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C75&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F75&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G75&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;/table&gt;&lt;h3 id="GeogLinearUnitSizeGeoKey"&gt;Requirements Class GeogLinearUnitSizeGeoKey&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogLinearUnitSizeGeoKey&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogLinearUnitSizeGeoKey.ID&lt;br/&gt;&lt;i&gt;The GeogLinearUnitSizeGeoKey SHALL have ID = 2053&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11748,14 +11752,14 @@
         <v>1852</v>
       </c>
       <c r="F76" s="9" t="str">
-        <f>Base_identifier&amp;C76&amp;"."&amp;E76</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogLinearUnitSizeGeoKey.type</v>
       </c>
       <c r="G76" s="9" t="s">
         <v>96</v>
       </c>
       <c r="H76" s="12" t="str">
-        <f>IF(C76=C75,"","&lt;/table&gt;&lt;h3 id="""&amp;C76&amp;"""&gt;Requirements Class "&amp;C76&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C76&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F76&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G76&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogLinearUnitSizeGeoKey.type&lt;br/&gt;&lt;i&gt;The GeogLinearUnitSizeGeoKey SHALL have type = DOUBLE&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11776,14 +11780,14 @@
         <v>1907</v>
       </c>
       <c r="F77" s="9" t="str">
-        <f>Base_identifier&amp;C77&amp;"."&amp;E77</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogLinearUnitSizeGeoKey.units</v>
       </c>
       <c r="G77" s="9" t="s">
         <v>97</v>
       </c>
       <c r="H77" s="12" t="str">
-        <f>IF(C77=C76,"","&lt;/table&gt;&lt;h3 id="""&amp;C77&amp;"""&gt;Requirements Class "&amp;C77&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C77&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F77&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G77&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogLinearUnitSizeGeoKey.units&lt;br/&gt;&lt;i&gt;The units of the GeogLinearUnitSizeGeoKey SHALL be meters&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11804,14 +11808,14 @@
         <v>1851</v>
       </c>
       <c r="F78" s="9" t="str">
-        <f>Base_identifier&amp;C78&amp;"."&amp;E78</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogAngularUnitsGeoKey.ID</v>
       </c>
       <c r="G78" s="9" t="s">
         <v>106</v>
       </c>
       <c r="H78" s="12" t="str">
-        <f>IF(C78=C77,"","&lt;/table&gt;&lt;h3 id="""&amp;C78&amp;"""&gt;Requirements Class "&amp;C78&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C78&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F78&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G78&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;/table&gt;&lt;h3 id="GeogAngularUnitsGeoKey"&gt;Requirements Class GeogAngularUnitsGeoKey&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogAngularUnitsGeoKey&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogAngularUnitsGeoKey.ID&lt;br/&gt;&lt;i&gt;The GeogAngularUnitsGeoKey SHALL have ID = 2054&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11832,14 +11836,14 @@
         <v>1852</v>
       </c>
       <c r="F79" s="9" t="str">
-        <f>Base_identifier&amp;C79&amp;"."&amp;E79</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogAngularUnitsGeoKey.type</v>
       </c>
       <c r="G79" s="9" t="s">
         <v>107</v>
       </c>
       <c r="H79" s="12" t="str">
-        <f>IF(C79=C78,"","&lt;/table&gt;&lt;h3 id="""&amp;C79&amp;"""&gt;Requirements Class "&amp;C79&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C79&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F79&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G79&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogAngularUnitsGeoKey.type&lt;br/&gt;&lt;i&gt;The GeogAngularUnitsGeoKey SHALL have type = SHORT&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11860,14 +11864,14 @@
         <v>1851</v>
       </c>
       <c r="F80" s="9" t="str">
-        <f>Base_identifier&amp;C80&amp;"."&amp;E80</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogAngularUnitSizeGeoKey.ID</v>
       </c>
       <c r="G80" s="9" t="s">
         <v>1954</v>
       </c>
       <c r="H80" s="12" t="str">
-        <f>IF(C80=C79,"","&lt;/table&gt;&lt;h3 id="""&amp;C80&amp;"""&gt;Requirements Class "&amp;C80&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C80&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F80&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G80&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;/table&gt;&lt;h3 id="GeogAngularUnitSizeGeoKey"&gt;Requirements Class GeogAngularUnitSizeGeoKey&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogAngularUnitSizeGeoKey&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogAngularUnitSizeGeoKey.ID&lt;br/&gt;&lt;i&gt;The GeogAngularUnitSizeGeoKey SHALL have ID = 2055&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11888,14 +11892,14 @@
         <v>1852</v>
       </c>
       <c r="F81" s="9" t="str">
-        <f>Base_identifier&amp;C81&amp;"."&amp;E81</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogAngularUnitSizeGeoKey.type</v>
       </c>
       <c r="G81" s="9" t="s">
         <v>1955</v>
       </c>
       <c r="H81" s="12" t="str">
-        <f>IF(C81=C80,"","&lt;/table&gt;&lt;h3 id="""&amp;C81&amp;"""&gt;Requirements Class "&amp;C81&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C81&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F81&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G81&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogAngularUnitSizeGeoKey.type&lt;br/&gt;&lt;i&gt;The GeogAngularUnitSizeGeoKey SHALL have type = DOUBLE&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11916,14 +11920,14 @@
         <v>1907</v>
       </c>
       <c r="F82" s="9" t="str">
-        <f>Base_identifier&amp;C82&amp;"."&amp;E82</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogAngularUnitSizeGeoKey.units</v>
       </c>
       <c r="G82" s="9" t="s">
         <v>1956</v>
       </c>
       <c r="H82" s="12" t="str">
-        <f>IF(C82=C81,"","&lt;/table&gt;&lt;h3 id="""&amp;C82&amp;"""&gt;Requirements Class "&amp;C82&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C82&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F82&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G82&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogAngularUnitSizeGeoKey.units&lt;br/&gt;&lt;i&gt;The units of the GeogAngularUnitSizeGeoKey SHALL be radians&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11944,14 +11948,14 @@
         <v>1898</v>
       </c>
       <c r="F83" s="9" t="str">
-        <f>Base_identifier&amp;C83&amp;"."&amp;E83</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogEllipsoidGeoKey.EPSGEllipsoid</v>
       </c>
       <c r="G83" s="9" t="s">
         <v>1962</v>
       </c>
       <c r="H83" s="12" t="str">
-        <f>IF(C83=C82,"","&lt;/table&gt;&lt;h3 id="""&amp;C83&amp;"""&gt;Requirements Class "&amp;C83&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C83&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F83&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G83&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;/table&gt;&lt;h3 id="GeogEllipsoidGeoKey"&gt;Requirements Class GeogEllipsoidGeoKey&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogEllipsoidGeoKey&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogEllipsoidGeoKey.EPSGEllipsoid&lt;br/&gt;&lt;i&gt;GeogEllipsoidGeoKey  values in the range 7000-7999 SHALL be EPSG Ellipsoid Codes&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -11972,14 +11976,14 @@
         <v>1851</v>
       </c>
       <c r="F84" s="9" t="str">
-        <f>Base_identifier&amp;C84&amp;"."&amp;E84</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogEllipsoidGeoKey.ID</v>
       </c>
       <c r="G84" s="9" t="s">
         <v>1957</v>
       </c>
       <c r="H84" s="12" t="str">
-        <f>IF(C84=C83,"","&lt;/table&gt;&lt;h3 id="""&amp;C84&amp;"""&gt;Requirements Class "&amp;C84&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C84&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F84&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G84&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogEllipsoidGeoKey.ID&lt;br/&gt;&lt;i&gt;The GeogEllipsoidGeoKey SHALL have ID = 2056&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12000,14 +12004,14 @@
         <v>1897</v>
       </c>
       <c r="F85" s="9" t="str">
-        <f>Base_identifier&amp;C85&amp;"."&amp;E85</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogEllipsoidGeoKey.obsolete</v>
       </c>
       <c r="G85" s="9" t="s">
         <v>1960</v>
       </c>
       <c r="H85" s="12" t="str">
-        <f>IF(C85=C84,"","&lt;/table&gt;&lt;h3 id="""&amp;C85&amp;"""&gt;Requirements Class "&amp;C85&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C85&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F85&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G85&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogEllipsoidGeoKey.obsolete&lt;br/&gt;&lt;i&gt;GeogEllipsoidGeoKey  values in the range 1-1000 SHALL be obsolete EPSG/POSC Datum Codes&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12028,14 +12032,14 @@
         <v>1890</v>
       </c>
       <c r="F86" s="9" t="str">
-        <f>Base_identifier&amp;C86&amp;"."&amp;E86</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogEllipsoidGeoKey.private</v>
       </c>
       <c r="G86" s="9" t="s">
         <v>1963</v>
       </c>
       <c r="H86" s="12" t="str">
-        <f>IF(C86=C85,"","&lt;/table&gt;&lt;h3 id="""&amp;C86&amp;"""&gt;Requirements Class "&amp;C86&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C86&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F86&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G86&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogEllipsoidGeoKey.private&lt;br/&gt;&lt;i&gt;GeogEllipsoidGeoKey  values in the range 32768-65535 SHALL be private&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12056,14 +12060,14 @@
         <v>1882</v>
       </c>
       <c r="F87" s="9" t="str">
-        <f>Base_identifier&amp;C87&amp;"."&amp;E87</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogEllipsoidGeoKey.reserved</v>
       </c>
       <c r="G87" s="9" t="s">
         <v>1961</v>
       </c>
       <c r="H87" s="12" t="str">
-        <f>IF(C87=C86,"","&lt;/table&gt;&lt;h3 id="""&amp;C87&amp;"""&gt;Requirements Class "&amp;C87&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C87&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F87&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G87&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogEllipsoidGeoKey.reserved&lt;br/&gt;&lt;i&gt;GeogEllipsoidGeoKey  values in the range 1001-6999 and 8000-32766 SHALL be reserved&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12084,14 +12088,14 @@
         <v>1852</v>
       </c>
       <c r="F88" s="9" t="str">
-        <f>Base_identifier&amp;C88&amp;"."&amp;E88</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogEllipsoidGeoKey.type</v>
       </c>
       <c r="G88" s="9" t="s">
         <v>1958</v>
       </c>
       <c r="H88" s="12" t="str">
-        <f>IF(C88=C87,"","&lt;/table&gt;&lt;h3 id="""&amp;C88&amp;"""&gt;Requirements Class "&amp;C88&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C88&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F88&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G88&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogEllipsoidGeoKey.type&lt;br/&gt;&lt;i&gt;The GeogEllipsoidGeoKey SHALL have type = SHORT&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12112,14 +12116,14 @@
         <v>1851</v>
       </c>
       <c r="F89" s="9" t="str">
-        <f>Base_identifier&amp;C89&amp;"."&amp;E89</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogSemiMajorAxisGeoKey.ID</v>
       </c>
       <c r="G89" s="9" t="s">
         <v>1964</v>
       </c>
       <c r="H89" s="12" t="str">
-        <f>IF(C89=C88,"","&lt;/table&gt;&lt;h3 id="""&amp;C89&amp;"""&gt;Requirements Class "&amp;C89&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C89&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F89&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G89&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;/table&gt;&lt;h3 id="GeogSemiMajorAxisGeoKey"&gt;Requirements Class GeogSemiMajorAxisGeoKey&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogSemiMajorAxisGeoKey&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogSemiMajorAxisGeoKey.ID&lt;br/&gt;&lt;i&gt;The GeogSemiMajorAxisGeoKey SHALL have ID = 2057&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12140,14 +12144,14 @@
         <v>1852</v>
       </c>
       <c r="F90" s="9" t="str">
-        <f>Base_identifier&amp;C90&amp;"."&amp;E90</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogSemiMajorAxisGeoKey.type</v>
       </c>
       <c r="G90" s="9" t="s">
         <v>1965</v>
       </c>
       <c r="H90" s="12" t="str">
-        <f>IF(C90=C89,"","&lt;/table&gt;&lt;h3 id="""&amp;C90&amp;"""&gt;Requirements Class "&amp;C90&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C90&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F90&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G90&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogSemiMajorAxisGeoKey.type&lt;br/&gt;&lt;i&gt;The GeogSemiMajorAxisGeoKey SHALL have type = DOUBLE&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12168,14 +12172,14 @@
         <v>1907</v>
       </c>
       <c r="F91" s="9" t="str">
-        <f>Base_identifier&amp;C91&amp;"."&amp;E91</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogSemiMajorAxisGeoKey.units</v>
       </c>
       <c r="G91" s="9" t="s">
         <v>1966</v>
       </c>
       <c r="H91" s="12" t="str">
-        <f>IF(C91=C90,"","&lt;/table&gt;&lt;h3 id="""&amp;C91&amp;"""&gt;Requirements Class "&amp;C91&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C91&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F91&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G91&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogSemiMajorAxisGeoKey.units&lt;br/&gt;&lt;i&gt;The units of the GeogSemiMajorAxisGeoKey SHALL be Geocentric CS linear Units&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12196,14 +12200,14 @@
         <v>1851</v>
       </c>
       <c r="F92" s="9" t="str">
-        <f>Base_identifier&amp;C92&amp;"."&amp;E92</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogSemiMinorAxisGeoKey.ID</v>
       </c>
       <c r="G92" s="9" t="s">
         <v>1967</v>
       </c>
       <c r="H92" s="12" t="str">
-        <f>IF(C92=C91,"","&lt;/table&gt;&lt;h3 id="""&amp;C92&amp;"""&gt;Requirements Class "&amp;C92&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C92&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F92&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G92&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;/table&gt;&lt;h3 id="GeogSemiMinorAxisGeoKey"&gt;Requirements Class GeogSemiMinorAxisGeoKey&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogSemiMinorAxisGeoKey&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogSemiMinorAxisGeoKey.ID&lt;br/&gt;&lt;i&gt;The GeogSemiMinorAxisGeoKey SHALL have ID = 2058&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12224,14 +12228,14 @@
         <v>1852</v>
       </c>
       <c r="F93" s="9" t="str">
-        <f>Base_identifier&amp;C93&amp;"."&amp;E93</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogSemiMinorAxisGeoKey.type</v>
       </c>
       <c r="G93" s="9" t="s">
         <v>1968</v>
       </c>
       <c r="H93" s="12" t="str">
-        <f>IF(C93=C92,"","&lt;/table&gt;&lt;h3 id="""&amp;C93&amp;"""&gt;Requirements Class "&amp;C93&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C93&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F93&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G93&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogSemiMinorAxisGeoKey.type&lt;br/&gt;&lt;i&gt;The GeogSemiMinorAxisGeoKey SHALL have type = DOUBLE&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12252,14 +12256,14 @@
         <v>1907</v>
       </c>
       <c r="F94" s="9" t="str">
-        <f>Base_identifier&amp;C94&amp;"."&amp;E94</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogSemiMinorAxisGeoKey.units</v>
       </c>
       <c r="G94" s="9" t="s">
         <v>1969</v>
       </c>
       <c r="H94" s="12" t="str">
-        <f>IF(C94=C93,"","&lt;/table&gt;&lt;h3 id="""&amp;C94&amp;"""&gt;Requirements Class "&amp;C94&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C94&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F94&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G94&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogSemiMinorAxisGeoKey.units&lt;br/&gt;&lt;i&gt;The units of the GeogSemiMinorAxisGeoKey HALL be Geocentric CS linear Units&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12280,14 +12284,14 @@
         <v>1851</v>
       </c>
       <c r="F95" s="9" t="str">
-        <f>Base_identifier&amp;C95&amp;"."&amp;E95</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogInvFlatteningGeoKey.ID</v>
       </c>
       <c r="G95" s="9" t="s">
         <v>1970</v>
       </c>
       <c r="H95" s="12" t="str">
-        <f>IF(C95=C94,"","&lt;/table&gt;&lt;h3 id="""&amp;C95&amp;"""&gt;Requirements Class "&amp;C95&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C95&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F95&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G95&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;/table&gt;&lt;h3 id="GeogInvFlatteningGeoKey"&gt;Requirements Class GeogInvFlatteningGeoKey&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogInvFlatteningGeoKey&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogInvFlatteningGeoKey.ID&lt;br/&gt;&lt;i&gt;The GeogInvFlatteningGeoKey SHALL have ID = 2059&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12308,14 +12312,14 @@
         <v>1852</v>
       </c>
       <c r="F96" s="9" t="str">
-        <f>Base_identifier&amp;C96&amp;"."&amp;E96</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogInvFlatteningGeoKey.type</v>
       </c>
       <c r="G96" s="9" t="s">
         <v>1971</v>
       </c>
       <c r="H96" s="12" t="str">
-        <f>IF(C96=C95,"","&lt;/table&gt;&lt;h3 id="""&amp;C96&amp;"""&gt;Requirements Class "&amp;C96&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C96&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F96&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G96&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogInvFlatteningGeoKey.type&lt;br/&gt;&lt;i&gt;The GeogInvFlatteningGeoKey SHALL have type = DOUBLE&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12336,14 +12340,14 @@
         <v>1851</v>
       </c>
       <c r="F97" s="9" t="str">
-        <f>Base_identifier&amp;C97&amp;"."&amp;E97</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogAzimuthUnitsGeoKey.ID</v>
       </c>
       <c r="G97" s="9" t="s">
         <v>1972</v>
       </c>
       <c r="H97" s="12" t="str">
-        <f>IF(C97=C96,"","&lt;/table&gt;&lt;h3 id="""&amp;C97&amp;"""&gt;Requirements Class "&amp;C97&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C97&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F97&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G97&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;/table&gt;&lt;h3 id="GeogAzimuthUnitsGeoKey"&gt;Requirements Class GeogAzimuthUnitsGeoKey&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogAzimuthUnitsGeoKey&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogAzimuthUnitsGeoKey.ID&lt;br/&gt;&lt;i&gt;The GeogAzimuthUnitsGeoKey SHALL have ID = 2060&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12364,14 +12368,14 @@
         <v>1852</v>
       </c>
       <c r="F98" s="9" t="str">
-        <f>Base_identifier&amp;C98&amp;"."&amp;E98</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeogAzimuthUnitsGeoKey.type</v>
       </c>
       <c r="G98" s="9" t="s">
         <v>1973</v>
       </c>
       <c r="H98" s="12" t="str">
-        <f>IF(C98=C97,"","&lt;/table&gt;&lt;h3 id="""&amp;C98&amp;"""&gt;Requirements Class "&amp;C98&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C98&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F98&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G98&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeogAzimuthUnitsGeoKey.type&lt;br/&gt;&lt;i&gt;The GeogAzimuthUnitsGeoKey SHALL have type = SHORT&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12392,14 +12396,14 @@
         <v>2014</v>
       </c>
       <c r="F99" s="9" t="str">
-        <f>Base_identifier&amp;C99&amp;"."&amp;E99</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/ProjectedCSTypeGeoKey.EPSGProjection</v>
       </c>
       <c r="G99" s="9" t="s">
         <v>1978</v>
       </c>
       <c r="H99" s="12" t="str">
-        <f>IF(C99=C98,"","&lt;/table&gt;&lt;h3 id="""&amp;C99&amp;"""&gt;Requirements Class "&amp;C99&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C99&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F99&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G99&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;/table&gt;&lt;h3 id="ProjectedCSTypeGeoKey"&gt;Requirements Class ProjectedCSTypeGeoKey&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/ProjectedCSTypeGeoKey&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/ProjectedCSTypeGeoKey.EPSGProjection&lt;br/&gt;&lt;i&gt;ProjectedCSTypeGeoKey  values in the range 20000-32760 SHALL be EPSG Projection System Codes&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12420,14 +12424,14 @@
         <v>1851</v>
       </c>
       <c r="F100" s="9" t="str">
-        <f>Base_identifier&amp;C100&amp;"."&amp;E100</f>
+        <f t="shared" si="4"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/ProjectedCSTypeGeoKey.ID</v>
       </c>
       <c r="G100" s="9" t="s">
         <v>1974</v>
       </c>
       <c r="H100" s="12" t="str">
-        <f>IF(C100=C99,"","&lt;/table&gt;&lt;h3 id="""&amp;C100&amp;"""&gt;Requirements Class "&amp;C100&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C100&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F100&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G100&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="5"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/ProjectedCSTypeGeoKey.ID&lt;br/&gt;&lt;i&gt;The ProjectedCSTypeGeoKey SHALL have ID = 3072&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12448,14 +12452,14 @@
         <v>2015</v>
       </c>
       <c r="F101" s="9" t="str">
-        <f>Base_identifier&amp;C101&amp;"."&amp;E101</f>
+        <f t="shared" ref="F101:F132" si="6">Base_identifier&amp;C101&amp;"."&amp;E101</f>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/ProjectedCSTypeGeoKey.KeyValues</v>
       </c>
       <c r="G101" s="9" t="s">
         <v>2033</v>
       </c>
       <c r="H101" s="12" t="str">
-        <f>IF(C101=C100,"","&lt;/table&gt;&lt;h3 id="""&amp;C101&amp;"""&gt;Requirements Class "&amp;C101&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C101&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F101&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G101&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" ref="H101:H132" si="7">IF(C101=C100,"","&lt;/table&gt;&lt;h3 id="""&amp;C101&amp;"""&gt;Requirements Class "&amp;C101&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C101&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F101&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G101&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/ProjectedCSTypeGeoKey.KeyValues&lt;br/&gt;&lt;i&gt;326zz – UTM Northern Hemisphere, 327zz – UTM Southern Hemisphere (Where zz is the UTM zone number), Other PCS allowed by this standard (in conformance with DGIWG Geodetic Codes and Parameters Registry) 12 Present only for cartographic data. In this case, GTModelTypeGeoKey = 1 and GeographicTypeGeoKey is absent&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12476,14 +12480,14 @@
         <v>1897</v>
       </c>
       <c r="F102" s="9" t="str">
-        <f>Base_identifier&amp;C102&amp;"."&amp;E102</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/ProjectedCSTypeGeoKey.obsolete</v>
       </c>
       <c r="G102" s="9" t="s">
         <v>1977</v>
       </c>
       <c r="H102" s="12" t="str">
-        <f>IF(C102=C101,"","&lt;/table&gt;&lt;h3 id="""&amp;C102&amp;"""&gt;Requirements Class "&amp;C102&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C102&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F102&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G102&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/ProjectedCSTypeGeoKey.obsolete&lt;br/&gt;&lt;i&gt;ProjectedCSTypeGeoKey  values in the range 1-1000 SHALL be obsolete EPSG/POSC Datum Codes&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12504,14 +12508,14 @@
         <v>1890</v>
       </c>
       <c r="F103" s="9" t="str">
-        <f>Base_identifier&amp;C103&amp;"."&amp;E103</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/ProjectedCSTypeGeoKey.private</v>
       </c>
       <c r="G103" s="9" t="s">
         <v>1979</v>
       </c>
       <c r="H103" s="12" t="str">
-        <f>IF(C103=C102,"","&lt;/table&gt;&lt;h3 id="""&amp;C103&amp;"""&gt;Requirements Class "&amp;C103&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C103&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F103&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G103&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/ProjectedCSTypeGeoKey.private&lt;br/&gt;&lt;i&gt;ProjectedCSTypeGeoKey  values in the range 32768-65535 SHALL be private&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12532,14 +12536,14 @@
         <v>1852</v>
       </c>
       <c r="F104" s="9" t="str">
-        <f>Base_identifier&amp;C104&amp;"."&amp;E104</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/ProjectedCSTypeGeoKey.type</v>
       </c>
       <c r="G104" s="9" t="s">
         <v>1975</v>
       </c>
       <c r="H104" s="12" t="str">
-        <f>IF(C104=C103,"","&lt;/table&gt;&lt;h3 id="""&amp;C104&amp;"""&gt;Requirements Class "&amp;C104&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C104&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F104&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G104&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/ProjectedCSTypeGeoKey.type&lt;br/&gt;&lt;i&gt;The ProjectedCSTypeGeoKey SHALL have type = SHORT&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12558,14 +12562,14 @@
         <v>1851</v>
       </c>
       <c r="F105" s="9" t="str">
-        <f>Base_identifier&amp;C105&amp;"."&amp;E105</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/PCSCitationGeoKey.ID</v>
       </c>
       <c r="G105" s="9" t="s">
         <v>1980</v>
       </c>
       <c r="H105" s="12" t="str">
-        <f>IF(C105=C104,"","&lt;/table&gt;&lt;h3 id="""&amp;C105&amp;"""&gt;Requirements Class "&amp;C105&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C105&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F105&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G105&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;/table&gt;&lt;h3 id="PCSCitationGeoKey"&gt;Requirements Class PCSCitationGeoKey&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/PCSCitationGeoKey&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/PCSCitationGeoKey.ID&lt;br/&gt;&lt;i&gt;The PCSCitationGeoKey SHALL have ID = 3073&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12584,14 +12588,14 @@
         <v>1852</v>
       </c>
       <c r="F106" s="9" t="str">
-        <f>Base_identifier&amp;C106&amp;"."&amp;E106</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/PCSCitationGeoKey.type</v>
       </c>
       <c r="G106" s="9" t="s">
         <v>1981</v>
       </c>
       <c r="H106" s="12" t="str">
-        <f>IF(C106=C105,"","&lt;/table&gt;&lt;h3 id="""&amp;C106&amp;"""&gt;Requirements Class "&amp;C106&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C106&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F106&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G106&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/PCSCitationGeoKey.type&lt;br/&gt;&lt;i&gt;The PCSCitationGeoKey SHALL have type = ASCII&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12610,14 +12614,14 @@
         <v>1898</v>
       </c>
       <c r="F107" s="9" t="str">
-        <f>Base_identifier&amp;C107&amp;"."&amp;E107</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/VerticalCSTypeGeoKey.EPSGEllipsoid</v>
       </c>
       <c r="G107" s="9" t="s">
         <v>1987</v>
       </c>
       <c r="H107" s="12" t="str">
-        <f>IF(C107=C106,"","&lt;/table&gt;&lt;h3 id="""&amp;C107&amp;"""&gt;Requirements Class "&amp;C107&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C107&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F107&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G107&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;/table&gt;&lt;h3 id="VerticalCSTypeGeoKey"&gt;Requirements Class VerticalCSTypeGeoKey&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VerticalCSTypeGeoKey&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VerticalCSTypeGeoKey.EPSGEllipsoid&lt;br/&gt;&lt;i&gt;VerticalCSTypeGeoKey  values in the range 5000-5099 SHALL be EPSG Ellipsoid Vertical CS Codes&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12636,14 +12640,14 @@
         <v>2019</v>
       </c>
       <c r="F108" s="9" t="str">
-        <f>Base_identifier&amp;C108&amp;"."&amp;E108</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/VerticalCSTypeGeoKey.EPSGOrthometric</v>
       </c>
       <c r="G108" s="9" t="s">
         <v>1988</v>
       </c>
       <c r="H108" s="12" t="str">
-        <f>IF(C108=C107,"","&lt;/table&gt;&lt;h3 id="""&amp;C108&amp;"""&gt;Requirements Class "&amp;C108&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C108&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F108&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G108&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VerticalCSTypeGeoKey.EPSGOrthometric&lt;br/&gt;&lt;i&gt;VerticalCSTypeGeoKey  values in the range 5100-5199 SHALL be EPSG Orthometric Vertical CS Codes&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12662,18 +12666,18 @@
         <v>1851</v>
       </c>
       <c r="F109" s="9" t="str">
-        <f>Base_identifier&amp;C109&amp;"."&amp;E109</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/VerticalCSTypeGeoKey.ID</v>
       </c>
       <c r="G109" s="9" t="s">
         <v>1982</v>
       </c>
       <c r="H109" s="12" t="str">
-        <f>IF(C109=C108,"","&lt;/table&gt;&lt;h3 id="""&amp;C109&amp;"""&gt;Requirements Class "&amp;C109&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C109&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F109&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G109&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VerticalCSTypeGeoKey.ID&lt;br/&gt;&lt;i&gt;The VerticalCSTypeGeoKey SHALL have ID = 4096&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="30">
+    <row r="110" spans="1:8" ht="45">
       <c r="A110" s="9" t="s">
         <v>1948</v>
       </c>
@@ -12688,14 +12692,14 @@
         <v>2015</v>
       </c>
       <c r="F110" s="9" t="str">
-        <f>Base_identifier&amp;C110&amp;"."&amp;E110</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/VerticalCSTypeGeoKey.KeyValues</v>
       </c>
       <c r="G110" s="9" t="s">
         <v>2034</v>
       </c>
       <c r="H110" s="12" t="str">
-        <f>IF(C110=C109,"","&lt;/table&gt;&lt;h3 id="""&amp;C110&amp;"""&gt;Requirements Class "&amp;C110&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C110&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F110&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G110&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VerticalCSTypeGeoKey.KeyValues&lt;br/&gt;&lt;i&gt;4979 (WGS84 3D ellipsoid), 5773 (EGM96), 3855 (EGM08), 5798 (EGM84), 5714 (MSL height), 5715 (MSL depth), 32767 for other Sounding datums idenfied in DGIWG Geodetic registry, or user defined Vertical CRS&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12714,14 +12718,14 @@
         <v>1890</v>
       </c>
       <c r="F111" s="9" t="str">
-        <f>Base_identifier&amp;C111&amp;"."&amp;E111</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/VerticalCSTypeGeoKey.private</v>
       </c>
       <c r="G111" s="9" t="s">
         <v>1989</v>
       </c>
       <c r="H111" s="12" t="str">
-        <f>IF(C111=C110,"","&lt;/table&gt;&lt;h3 id="""&amp;C111&amp;"""&gt;Requirements Class "&amp;C111&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C111&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F111&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G111&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VerticalCSTypeGeoKey.private&lt;br/&gt;&lt;i&gt;VerticalCSTypeGeoKey  values in the range 32768-65535 SHALL be private&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12740,14 +12744,14 @@
         <v>1882</v>
       </c>
       <c r="F112" s="9" t="str">
-        <f>Base_identifier&amp;C112&amp;"."&amp;E112</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/VerticalCSTypeGeoKey.reserved</v>
       </c>
       <c r="G112" s="9" t="s">
         <v>1985</v>
       </c>
       <c r="H112" s="12" t="str">
-        <f>IF(C112=C111,"","&lt;/table&gt;&lt;h3 id="""&amp;C112&amp;"""&gt;Requirements Class "&amp;C112&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C112&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F112&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G112&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VerticalCSTypeGeoKey.reserved&lt;br/&gt;&lt;i&gt;VerticalCSTypeGeoKey  values in the range 1-4999 and 6000-32766 SHALL be reserved&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12766,14 +12770,14 @@
         <v>2018</v>
       </c>
       <c r="F113" s="9" t="str">
-        <f>Base_identifier&amp;C113&amp;"."&amp;E113</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/VerticalCSTypeGeoKey.reservedEPSG</v>
       </c>
       <c r="G113" s="9" t="s">
         <v>1986</v>
       </c>
       <c r="H113" s="12" t="str">
-        <f>IF(C113=C112,"","&lt;/table&gt;&lt;h3 id="""&amp;C113&amp;"""&gt;Requirements Class "&amp;C113&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C113&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F113&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G113&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VerticalCSTypeGeoKey.reservedEPSG&lt;br/&gt;&lt;i&gt;VerticalCSTypeGeoKey  values in the range 5200-5999 SHALL be reserved EPSG&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12792,14 +12796,14 @@
         <v>1852</v>
       </c>
       <c r="F114" s="9" t="str">
-        <f>Base_identifier&amp;C114&amp;"."&amp;E114</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/VerticalCSTypeGeoKey.type</v>
       </c>
       <c r="G114" s="9" t="s">
         <v>1983</v>
       </c>
       <c r="H114" s="12" t="str">
-        <f>IF(C114=C113,"","&lt;/table&gt;&lt;h3 id="""&amp;C114&amp;"""&gt;Requirements Class "&amp;C114&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C114&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F114&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G114&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VerticalCSTypeGeoKey.type&lt;br/&gt;&lt;i&gt;The VerticalCSTypeGeoKey SHALL have type = SHORT&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12818,18 +12822,18 @@
         <v>1851</v>
       </c>
       <c r="F115" s="9" t="str">
-        <f>Base_identifier&amp;C115&amp;"."&amp;E115</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/VerticalCitationGeoKey.ID</v>
       </c>
       <c r="G115" s="9" t="s">
         <v>1990</v>
       </c>
       <c r="H115" s="12" t="str">
-        <f>IF(C115=C114,"","&lt;/table&gt;&lt;h3 id="""&amp;C115&amp;"""&gt;Requirements Class "&amp;C115&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C115&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F115&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G115&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;/table&gt;&lt;h3 id="VerticalCitationGeoKey"&gt;Requirements Class VerticalCitationGeoKey&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VerticalCitationGeoKey&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VerticalCitationGeoKey.ID&lt;br/&gt;&lt;i&gt;The VerticalCitationGeoKey SHALL have ID = 4097&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="30">
+    <row r="116" spans="1:8" ht="45">
       <c r="A116" s="9" t="s">
         <v>1948</v>
       </c>
@@ -12844,14 +12848,14 @@
         <v>2015</v>
       </c>
       <c r="F116" s="9" t="str">
-        <f>Base_identifier&amp;C116&amp;"."&amp;E116</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/VerticalCitationGeoKey.KeyValues</v>
       </c>
       <c r="G116" s="9" t="s">
         <v>1992</v>
       </c>
       <c r="H116" s="12" t="str">
-        <f>IF(C116=C115,"","&lt;/table&gt;&lt;h3 id="""&amp;C116&amp;"""&gt;Requirements Class "&amp;C116&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C116&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F116&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G116&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VerticalCitationGeoKey.KeyValues&lt;br/&gt;&lt;i&gt;WGS84 Ellipsoid, EGM84, EGM96, EGM2008, MSL height, MSL depth , or the name of the Sounding datum identified in DGIWG Geodetic registry (S-1 to S-40), or description os user-defined vertical CRS&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12870,14 +12874,14 @@
         <v>1852</v>
       </c>
       <c r="F117" s="9" t="str">
-        <f>Base_identifier&amp;C117&amp;"."&amp;E117</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/VerticalCitationGeoKey.type</v>
       </c>
       <c r="G117" s="9" t="s">
         <v>1991</v>
       </c>
       <c r="H117" s="12" t="str">
-        <f>IF(C117=C116,"","&lt;/table&gt;&lt;h3 id="""&amp;C117&amp;"""&gt;Requirements Class "&amp;C117&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C117&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F117&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G117&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VerticalCitationGeoKey.type&lt;br/&gt;&lt;i&gt;The VerticalCitationGeoKey SHALL have type = ASCII&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12896,14 +12900,14 @@
         <v>1851</v>
       </c>
       <c r="F118" s="9" t="str">
-        <f>Base_identifier&amp;C118&amp;"."&amp;E118</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/VerticalDatumGeoKey.ID</v>
       </c>
       <c r="G118" s="9" t="s">
         <v>1993</v>
       </c>
       <c r="H118" s="12" t="str">
-        <f>IF(C118=C117,"","&lt;/table&gt;&lt;h3 id="""&amp;C118&amp;"""&gt;Requirements Class "&amp;C118&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C118&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F118&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G118&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;/table&gt;&lt;h3 id="VerticalDatumGeoKey"&gt;Requirements Class VerticalDatumGeoKey&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VerticalDatumGeoKey&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VerticalDatumGeoKey.ID&lt;br/&gt;&lt;i&gt;The VerticalDatumGeoKey SHALL have ID = 4098&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12922,14 +12926,14 @@
         <v>1890</v>
       </c>
       <c r="F119" s="9" t="str">
-        <f>Base_identifier&amp;C119&amp;"."&amp;E119</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/VerticalDatumGeoKey.private</v>
       </c>
       <c r="G119" s="9" t="s">
         <v>1998</v>
       </c>
       <c r="H119" s="12" t="str">
-        <f>IF(C119=C118,"","&lt;/table&gt;&lt;h3 id="""&amp;C119&amp;"""&gt;Requirements Class "&amp;C119&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C119&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F119&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G119&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VerticalDatumGeoKey.private&lt;br/&gt;&lt;i&gt;VerticalDatumGeoKey  values in the range 32768-65535 SHALL be private&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -12948,18 +12952,18 @@
         <v>1882</v>
       </c>
       <c r="F120" s="9" t="str">
-        <f>Base_identifier&amp;C120&amp;"."&amp;E120</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/VerticalDatumGeoKey.reserved</v>
       </c>
       <c r="G120" s="9" t="s">
         <v>1997</v>
       </c>
       <c r="H120" s="12" t="str">
-        <f>IF(C120=C119,"","&lt;/table&gt;&lt;h3 id="""&amp;C120&amp;"""&gt;Requirements Class "&amp;C120&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C120&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F120&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G120&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VerticalDatumGeoKey.reserved&lt;br/&gt;&lt;i&gt;VerticalDatumGeoKey  values in the range 16384-32766 SHALL be reserved&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="45">
+    <row r="121" spans="1:8" ht="30">
       <c r="A121" s="9" t="s">
         <v>1953</v>
       </c>
@@ -12974,14 +12978,14 @@
         <v>1852</v>
       </c>
       <c r="F121" s="9" t="str">
-        <f>Base_identifier&amp;C121&amp;"."&amp;E121</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/VerticalDatumGeoKey.type</v>
       </c>
       <c r="G121" s="9" t="s">
         <v>1994</v>
       </c>
       <c r="H121" s="12" t="str">
-        <f>IF(C121=C120,"","&lt;/table&gt;&lt;h3 id="""&amp;C121&amp;"""&gt;Requirements Class "&amp;C121&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C121&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F121&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G121&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VerticalDatumGeoKey.type&lt;br/&gt;&lt;i&gt;The VerticalDatumGeoKey SHALL have type = SHORT&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -13000,18 +13004,18 @@
         <v>2022</v>
       </c>
       <c r="F122" s="9" t="str">
-        <f>Base_identifier&amp;C122&amp;"."&amp;E122</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/VerticalDatumGeoKey.VertDatum</v>
       </c>
       <c r="G122" s="9" t="s">
         <v>1996</v>
       </c>
       <c r="H122" s="12" t="str">
-        <f>IF(C122=C121,"","&lt;/table&gt;&lt;h3 id="""&amp;C122&amp;"""&gt;Requirements Class "&amp;C122&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C122&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F122&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G122&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VerticalDatumGeoKey.VertDatum&lt;br/&gt;&lt;i&gt;VerticalDatumGeoKey  values in the range 1-16383 SHALL be Vertical Datum Codes&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="45">
+    <row r="123" spans="1:8" ht="30">
       <c r="A123" s="9" t="s">
         <v>95</v>
       </c>
@@ -13026,18 +13030,18 @@
         <v>1910</v>
       </c>
       <c r="F123" s="9" t="str">
-        <f>Base_identifier&amp;C123&amp;"."&amp;E123</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/VerticalUnitsGeoKey.angular</v>
       </c>
       <c r="G123" s="9" t="s">
         <v>2004</v>
       </c>
       <c r="H123" s="12" t="str">
-        <f>IF(C123=C122,"","&lt;/table&gt;&lt;h3 id="""&amp;C123&amp;"""&gt;Requirements Class "&amp;C123&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C123&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F123&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G123&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;/table&gt;&lt;h3 id="VerticalUnitsGeoKey"&gt;Requirements Class VerticalUnitsGeoKey&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VerticalUnitsGeoKey&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VerticalUnitsGeoKey.angular&lt;br/&gt;&lt;i&gt;VerticalUnitsGeoKey values in the range 9100-9199 SHALL be EPSG angular units&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="75">
+    <row r="124" spans="1:8" ht="30">
       <c r="A124" s="9" t="s">
         <v>1953</v>
       </c>
@@ -13052,14 +13056,14 @@
         <v>1851</v>
       </c>
       <c r="F124" s="9" t="str">
-        <f>Base_identifier&amp;C124&amp;"."&amp;E124</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/VerticalUnitsGeoKey.ID</v>
       </c>
       <c r="G124" s="9" t="s">
         <v>1999</v>
       </c>
       <c r="H124" s="12" t="str">
-        <f>IF(C124=C123,"","&lt;/table&gt;&lt;h3 id="""&amp;C124&amp;"""&gt;Requirements Class "&amp;C124&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C124&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F124&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G124&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VerticalUnitsGeoKey.ID&lt;br/&gt;&lt;i&gt;The VerticalUnitsGeoKey SHALL have ID = 4099&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -13078,18 +13082,18 @@
         <v>2015</v>
       </c>
       <c r="F125" s="9" t="str">
-        <f>Base_identifier&amp;C125&amp;"."&amp;E125</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/VerticalUnitsGeoKey.KeyValues</v>
       </c>
       <c r="G125" s="9" t="s">
         <v>2006</v>
       </c>
       <c r="H125" s="12" t="str">
-        <f>IF(C125=C124,"","&lt;/table&gt;&lt;h3 id="""&amp;C125&amp;"""&gt;Requirements Class "&amp;C125&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C125&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F125&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G125&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VerticalUnitsGeoKey.KeyValues&lt;br/&gt;&lt;i&gt;9001 (meaning Linear_Meter) &lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="45">
+    <row r="126" spans="1:8" ht="30">
       <c r="A126" s="9" t="s">
         <v>95</v>
       </c>
@@ -13104,18 +13108,18 @@
         <v>1909</v>
       </c>
       <c r="F126" s="9" t="str">
-        <f>Base_identifier&amp;C126&amp;"."&amp;E126</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/VerticalUnitsGeoKey.linear</v>
       </c>
       <c r="G126" s="9" t="s">
         <v>2003</v>
       </c>
       <c r="H126" s="12" t="str">
-        <f>IF(C126=C125,"","&lt;/table&gt;&lt;h3 id="""&amp;C126&amp;"""&gt;Requirements Class "&amp;C126&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C126&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F126&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G126&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VerticalUnitsGeoKey.linear&lt;br/&gt;&lt;i&gt;VerticalUnitsGeoKey values in the range 9000-9099 SHALL be EPSG linear units&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="45">
+    <row r="127" spans="1:8" ht="30">
       <c r="A127" s="9" t="s">
         <v>95</v>
       </c>
@@ -13130,14 +13134,14 @@
         <v>1897</v>
       </c>
       <c r="F127" s="9" t="str">
-        <f>Base_identifier&amp;C127&amp;"."&amp;E127</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/VerticalUnitsGeoKey.obsolete</v>
       </c>
       <c r="G127" s="9" t="s">
         <v>2001</v>
       </c>
       <c r="H127" s="12" t="str">
-        <f>IF(C127=C126,"","&lt;/table&gt;&lt;h3 id="""&amp;C127&amp;"""&gt;Requirements Class "&amp;C127&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C127&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F127&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G127&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VerticalUnitsGeoKey.obsolete&lt;br/&gt;&lt;i&gt;VerticalUnitsGeoKey values in the range 1-2000 SHALL be obsolete GeoTIFF Codes&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -13156,14 +13160,14 @@
         <v>1890</v>
       </c>
       <c r="F128" s="9" t="str">
-        <f>Base_identifier&amp;C128&amp;"."&amp;E128</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/VerticalUnitsGeoKey.private</v>
       </c>
       <c r="G128" s="9" t="s">
         <v>2005</v>
       </c>
       <c r="H128" s="12" t="str">
-        <f>IF(C128=C127,"","&lt;/table&gt;&lt;h3 id="""&amp;C128&amp;"""&gt;Requirements Class "&amp;C128&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C128&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F128&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G128&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VerticalUnitsGeoKey.private&lt;br/&gt;&lt;i&gt;VerticalUnitsGeoKey values in the range 32768-65535 SHALL be private&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -13182,14 +13186,14 @@
         <v>1882</v>
       </c>
       <c r="F129" s="9" t="str">
-        <f>Base_identifier&amp;C129&amp;"."&amp;E129</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/VerticalUnitsGeoKey.reserved</v>
       </c>
       <c r="G129" s="9" t="s">
         <v>2002</v>
       </c>
       <c r="H129" s="12" t="str">
-        <f>IF(C129=C128,"","&lt;/table&gt;&lt;h3 id="""&amp;C129&amp;"""&gt;Requirements Class "&amp;C129&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C129&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F129&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G129&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VerticalUnitsGeoKey.reserved&lt;br/&gt;&lt;i&gt;VerticalUnitsGeoKey values in the range 2001-8999 SHALL be reserved&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -13208,14 +13212,14 @@
         <v>1852</v>
       </c>
       <c r="F130" s="9" t="str">
-        <f>Base_identifier&amp;C130&amp;"."&amp;E130</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/VerticalUnitsGeoKey.type</v>
       </c>
       <c r="G130" s="9" t="s">
         <v>2000</v>
       </c>
       <c r="H130" s="12" t="str">
-        <f>IF(C130=C129,"","&lt;/table&gt;&lt;h3 id="""&amp;C130&amp;"""&gt;Requirements Class "&amp;C130&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C130&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F130&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G130&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VerticalUnitsGeoKey.type&lt;br/&gt;&lt;i&gt;The VerticalUnitsGeoKey SHALL have type = SHORT&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -13232,14 +13236,14 @@
         <v>1904</v>
       </c>
       <c r="F131" s="9" t="str">
-        <f>Base_identifier&amp;C131&amp;"."&amp;E131</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeodeticDatumGeoKey.ArchaicDatum</v>
       </c>
       <c r="G131" s="9" t="s">
         <v>83</v>
       </c>
       <c r="H131" s="12" t="str">
-        <f>IF(C131=C130,"","&lt;/table&gt;&lt;h3 id="""&amp;C131&amp;"""&gt;Requirements Class "&amp;C131&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C131&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F131&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G131&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;/table&gt;&lt;h3 id="GeodeticDatumGeoKey"&gt;Requirements Class GeodeticDatumGeoKey&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeodeticDatumGeoKey&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeodeticDatumGeoKey.ArchaicDatum&lt;br/&gt;&lt;i&gt;GeodeticDatumGeoKey values in the range 6900-6999 SHALL be Archaic Datum&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -13256,14 +13260,14 @@
         <v>1899</v>
       </c>
       <c r="F132" s="9" t="str">
-        <f>Base_identifier&amp;C132&amp;"."&amp;E132</f>
+        <f t="shared" si="6"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeodeticDatumGeoKey.EPSGDatum</v>
       </c>
       <c r="G132" s="9" t="s">
         <v>80</v>
       </c>
       <c r="H132" s="12" t="str">
-        <f>IF(C132=C131,"","&lt;/table&gt;&lt;h3 id="""&amp;C132&amp;"""&gt;Requirements Class "&amp;C132&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C132&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F132&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G132&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="7"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeodeticDatumGeoKey.EPSGDatum&lt;br/&gt;&lt;i&gt;GeodeticDatumGeoKey values in the range 6200-6999 SHALL be EPSG Datum Based on EPSG Datum&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -13280,14 +13284,14 @@
         <v>1898</v>
       </c>
       <c r="F133" s="9" t="str">
-        <f>Base_identifier&amp;C133&amp;"."&amp;E133</f>
+        <f t="shared" ref="F133:F164" si="8">Base_identifier&amp;C133&amp;"."&amp;E133</f>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeodeticDatumGeoKey.EPSGEllipsoid</v>
       </c>
       <c r="G133" s="9" t="s">
         <v>79</v>
       </c>
       <c r="H133" s="12" t="str">
-        <f>IF(C133=C132,"","&lt;/table&gt;&lt;h3 id="""&amp;C133&amp;"""&gt;Requirements Class "&amp;C133&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C133&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F133&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G133&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" ref="H133:H164" si="9">IF(C133=C132,"","&lt;/table&gt;&lt;h3 id="""&amp;C133&amp;"""&gt;Requirements Class "&amp;C133&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C133&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F133&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G133&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeodeticDatumGeoKey.EPSGEllipsoid&lt;br/&gt;&lt;i&gt;GeodeticDatumGeoKey values in the range 6000-6199 SHALL be EPSG Datum Based on Ellipsoid only&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -13304,14 +13308,14 @@
         <v>1897</v>
       </c>
       <c r="F134" s="9" t="str">
-        <f>Base_identifier&amp;C134&amp;"."&amp;E134</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeodeticDatumGeoKey.obsolete</v>
       </c>
       <c r="G134" s="9" t="s">
         <v>76</v>
       </c>
       <c r="H134" s="12" t="str">
-        <f>IF(C134=C133,"","&lt;/table&gt;&lt;h3 id="""&amp;C134&amp;"""&gt;Requirements Class "&amp;C134&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C134&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F134&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G134&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeodeticDatumGeoKey.obsolete&lt;br/&gt;&lt;i&gt;GeodeticDatumGeoKey values in the range 1-1000 SHALL be obsolete EPSG/POSC Datum Codes&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -13328,18 +13332,18 @@
         <v>1890</v>
       </c>
       <c r="F135" s="9" t="str">
-        <f>Base_identifier&amp;C135&amp;"."&amp;E135</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeodeticDatumGeoKey.private</v>
       </c>
       <c r="G135" s="9" t="s">
         <v>84</v>
       </c>
       <c r="H135" s="12" t="str">
-        <f>IF(C135=C134,"","&lt;/table&gt;&lt;h3 id="""&amp;C135&amp;"""&gt;Requirements Class "&amp;C135&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C135&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F135&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G135&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeodeticDatumGeoKey.private&lt;br/&gt;&lt;i&gt;GeodeticDatumGeoKey values in the range 32768-65535 SHALL be private&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="45">
+    <row r="136" spans="1:8" ht="30">
       <c r="A136" s="9" t="s">
         <v>81</v>
       </c>
@@ -13352,14 +13356,14 @@
         <v>1882</v>
       </c>
       <c r="F136" s="9" t="str">
-        <f>Base_identifier&amp;C136&amp;"."&amp;E136</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeodeticDatumGeoKey.reserved</v>
       </c>
       <c r="G136" s="9" t="s">
         <v>78</v>
       </c>
       <c r="H136" s="12" t="str">
-        <f>IF(C136=C135,"","&lt;/table&gt;&lt;h3 id="""&amp;C136&amp;"""&gt;Requirements Class "&amp;C136&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C136&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F136&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G136&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeodeticDatumGeoKey.reserved&lt;br/&gt;&lt;i&gt;GeodeticDatumGeoKey values in the range 1001-5999 and 7000-32766 SHALL be reserved&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -13376,14 +13380,14 @@
         <v>1903</v>
       </c>
       <c r="F137" s="9" t="str">
-        <f>Base_identifier&amp;C137&amp;"."&amp;E137</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeodeticDatumGeoKey.WGSDatum</v>
       </c>
       <c r="G137" s="9" t="s">
         <v>82</v>
       </c>
       <c r="H137" s="12" t="str">
-        <f>IF(C137=C136,"","&lt;/table&gt;&lt;h3 id="""&amp;C137&amp;"""&gt;Requirements Class "&amp;C137&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C137&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F137&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G137&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeodeticDatumGeoKey.WGSDatum&lt;br/&gt;&lt;i&gt;GeodeticDatumGeoKey values in the range 6322-6327 SHALL be WGS Datum&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -13400,14 +13404,14 @@
         <v>1853</v>
       </c>
       <c r="F138" s="9" t="str">
-        <f>Base_identifier&amp;C138&amp;"."&amp;E138</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeoDoubleParamsTag.count</v>
       </c>
       <c r="G138" s="9" t="s">
         <v>2025</v>
       </c>
       <c r="H138" s="12" t="str">
-        <f>IF(C138=C137,"","&lt;/table&gt;&lt;h3 id="""&amp;C138&amp;"""&gt;Requirements Class "&amp;C138&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C138&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F138&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G138&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;/table&gt;&lt;h3 id="GeoDoubleParamsTag"&gt;Requirements Class GeoDoubleParamsTag&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoDoubleParamsTag&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoDoubleParamsTag.count&lt;br/&gt;&lt;i&gt;The GeoDoubleParamsTag MAY hold any number of key parameters with type = double. (May not be necessary, the same as keyentry.count) &lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -13424,14 +13428,14 @@
         <v>1851</v>
       </c>
       <c r="F139" s="9" t="str">
-        <f>Base_identifier&amp;C139&amp;"."&amp;E139</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeoDoubleParamsTag.ID</v>
       </c>
       <c r="G139" s="9" t="s">
         <v>10</v>
       </c>
       <c r="H139" s="12" t="str">
-        <f>IF(C139=C138,"","&lt;/table&gt;&lt;h3 id="""&amp;C139&amp;"""&gt;Requirements Class "&amp;C139&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C139&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F139&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G139&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoDoubleParamsTag.ID&lt;br/&gt;&lt;i&gt;The GeoDoubleParamsTag SHALL have ID = 34736&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -13448,14 +13452,14 @@
         <v>1852</v>
       </c>
       <c r="F140" s="9" t="str">
-        <f>Base_identifier&amp;C140&amp;"."&amp;E140</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeoDoubleParamsTag.type</v>
       </c>
       <c r="G140" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H140" s="12" t="str">
-        <f>IF(C140=C139,"","&lt;/table&gt;&lt;h3 id="""&amp;C140&amp;"""&gt;Requirements Class "&amp;C140&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C140&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F140&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G140&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoDoubleParamsTag.type&lt;br/&gt;&lt;i&gt;The GeoDoubleParamsTag SHALL have type = DOUBLE (IEEE Double Precision)&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -13472,14 +13476,14 @@
         <v>1883</v>
       </c>
       <c r="F141" s="9" t="str">
-        <f>Base_identifier&amp;C141&amp;"."&amp;E141</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyRange.configuration</v>
       </c>
       <c r="G141" s="9" t="s">
         <v>44</v>
       </c>
       <c r="H141" s="12" t="str">
-        <f>IF(C141=C140,"","&lt;/table&gt;&lt;h3 id="""&amp;C141&amp;"""&gt;Requirements Class "&amp;C141&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C141&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F141&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G141&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;/table&gt;&lt;h3 id="GeoKeyRange"&gt;Requirements Class GeoKeyRange&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyRange&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyRange.configuration&lt;br/&gt;&lt;i&gt;GeoKey ID's in the range 1024-2047 SHALL be GeoTIFF Configuration Keys&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -13496,18 +13500,18 @@
         <v>1884</v>
       </c>
       <c r="F142" s="9" t="str">
-        <f>Base_identifier&amp;C142&amp;"."&amp;E142</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyRange.geographic</v>
       </c>
       <c r="G142" s="9" t="s">
         <v>45</v>
       </c>
       <c r="H142" s="12" t="str">
-        <f>IF(C142=C141,"","&lt;/table&gt;&lt;h3 id="""&amp;C142&amp;"""&gt;Requirements Class "&amp;C142&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C142&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F142&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G142&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyRange.geographic&lt;br/&gt;&lt;i&gt;GeoKey ID's in the range 2048-3071 SHALL be Geographic/Geocentric Coordinate System Parameter Keys&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="143" spans="1:8" ht="45">
+    <row r="143" spans="1:8" ht="30">
       <c r="A143" s="9" t="s">
         <v>51</v>
       </c>
@@ -13520,14 +13524,14 @@
         <v>1885</v>
       </c>
       <c r="F143" s="9" t="str">
-        <f>Base_identifier&amp;C143&amp;"."&amp;E143</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyRange.projected</v>
       </c>
       <c r="G143" s="9" t="s">
         <v>46</v>
       </c>
       <c r="H143" s="12" t="str">
-        <f>IF(C143=C142,"","&lt;/table&gt;&lt;h3 id="""&amp;C143&amp;"""&gt;Requirements Class "&amp;C143&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C143&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F143&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G143&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyRange.projected&lt;br/&gt;&lt;i&gt;GeoKey ID's in the range 3072-4095 SHALL be Projected Coordinate System Parameter Keys&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -13544,14 +13548,14 @@
         <v>1882</v>
       </c>
       <c r="F144" s="9" t="str">
-        <f>Base_identifier&amp;C144&amp;"."&amp;E144</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyRange.reserved</v>
       </c>
       <c r="G144" s="9" t="s">
         <v>43</v>
       </c>
       <c r="H144" s="12" t="str">
-        <f>IF(C144=C143,"","&lt;/table&gt;&lt;h3 id="""&amp;C144&amp;"""&gt;Requirements Class "&amp;C144&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C144&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F144&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G144&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyRange.reserved&lt;br/&gt;&lt;i&gt;GeoKey ID's in the range 0-1023 and 5120-32767 SHALL be reserved&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -13568,14 +13572,14 @@
         <v>1882</v>
       </c>
       <c r="F145" s="9" t="str">
-        <f>Base_identifier&amp;C145&amp;"."&amp;E145</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyRange.reserved</v>
       </c>
       <c r="G145" s="9" t="s">
         <v>47</v>
       </c>
       <c r="H145" s="12" t="str">
-        <f>IF(C145=C144,"","&lt;/table&gt;&lt;h3 id="""&amp;C145&amp;"""&gt;Requirements Class "&amp;C145&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C145&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F145&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G145&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyRange.reserved&lt;br/&gt;&lt;i&gt;GeoKey ID's in the range 4096-5119 SHALL be Vertical Coordinate System Parameter Keys&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -13592,14 +13596,14 @@
         <v>1882</v>
       </c>
       <c r="F146" s="9" t="str">
-        <f>Base_identifier&amp;C146&amp;"."&amp;E146</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyRange.reserved</v>
       </c>
       <c r="G146" s="9" t="s">
         <v>48</v>
       </c>
       <c r="H146" s="12" t="str">
-        <f>IF(C146=C145,"","&lt;/table&gt;&lt;h3 id="""&amp;C146&amp;"""&gt;Requirements Class "&amp;C146&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C146&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F146&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G146&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/GeoKeyRange.reserved&lt;br/&gt;&lt;i&gt;GeoKey ID's in the range 32768-65535 SHALL be for private use&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -13616,14 +13620,14 @@
         <v>1853</v>
       </c>
       <c r="F147" s="9" t="str">
-        <f>Base_identifier&amp;C147&amp;"."&amp;E147</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/IntergraphMatrixTag.count</v>
       </c>
       <c r="G147" s="9" t="s">
         <v>41</v>
       </c>
       <c r="H147" s="12" t="str">
-        <f>IF(C147=C146,"","&lt;/table&gt;&lt;h3 id="""&amp;C147&amp;"""&gt;Requirements Class "&amp;C147&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C147&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F147&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G147&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;/table&gt;&lt;h3 id="IntergraphMatrixTag"&gt;Requirements Class IntergraphMatrixTag&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/IntergraphMatrixTag&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/IntergraphMatrixTag.count&lt;br/&gt;&lt;i&gt;The IntergraphMatrixTag SHALL hold sixteen or seventeen values &lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -13640,18 +13644,18 @@
         <v>1880</v>
       </c>
       <c r="F148" s="9" t="str">
-        <f>Base_identifier&amp;C148&amp;"."&amp;E148</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/IntergraphMatrixTag.deprecated</v>
       </c>
       <c r="G148" s="9" t="s">
         <v>42</v>
       </c>
       <c r="H148" s="12" t="str">
-        <f>IF(C148=C147,"","&lt;/table&gt;&lt;h3 id="""&amp;C148&amp;"""&gt;Requirements Class "&amp;C148&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C148&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F148&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G148&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/IntergraphMatrixTag.deprecated&lt;br/&gt;&lt;i&gt;The IntergraphMatrixTag SHALL not be used&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="149" spans="1:8" ht="60">
+    <row r="149" spans="1:8" ht="30">
       <c r="A149" s="9" t="s">
         <v>24</v>
       </c>
@@ -13664,14 +13668,14 @@
         <v>1851</v>
       </c>
       <c r="F149" s="9" t="str">
-        <f>Base_identifier&amp;C149&amp;"."&amp;E149</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/IntergraphMatrixTag.ID</v>
       </c>
       <c r="G149" s="9" t="s">
         <v>40</v>
       </c>
       <c r="H149" s="12" t="str">
-        <f>IF(C149=C148,"","&lt;/table&gt;&lt;h3 id="""&amp;C149&amp;"""&gt;Requirements Class "&amp;C149&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C149&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F149&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G149&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/IntergraphMatrixTag.ID&lt;br/&gt;&lt;i&gt;The IntergraphMatrixTag SHALL have ID = 33920&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -13688,14 +13692,14 @@
         <v>1852</v>
       </c>
       <c r="F150" s="9" t="str">
-        <f>Base_identifier&amp;C150&amp;"."&amp;E150</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/IntergraphMatrixTag.type</v>
       </c>
       <c r="G150" s="9" t="s">
         <v>39</v>
       </c>
       <c r="H150" s="12" t="str">
-        <f>IF(C150=C149,"","&lt;/table&gt;&lt;h3 id="""&amp;C150&amp;"""&gt;Requirements Class "&amp;C150&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C150&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F150&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G150&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/IntergraphMatrixTag.type&lt;br/&gt;&lt;i&gt;The IntergraphMatrixTag SHALL have type = DOUBLE&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -13714,14 +13718,14 @@
         <v>1853</v>
       </c>
       <c r="F151" s="9" t="str">
-        <f>Base_identifier&amp;C151&amp;"."&amp;E151</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/KeyEntrySet.count</v>
       </c>
       <c r="G151" s="10" t="s">
         <v>2029</v>
       </c>
       <c r="H151" s="12" t="str">
-        <f>IF(C151=C150,"","&lt;/table&gt;&lt;h3 id="""&amp;C151&amp;"""&gt;Requirements Class "&amp;C151&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C151&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F151&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G151&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;/table&gt;&lt;h3 id="KeyEntrySet"&gt;Requirements Class KeyEntrySet&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/KeyEntrySet&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/KeyEntrySet.count&lt;br/&gt;&lt;i&gt;The third unsigned short integer in each Key Entry Set SHALL hold the number of values in the key (the Count). If TIFFTagLocation=0,  Count=1 is implied.&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -13740,18 +13744,18 @@
         <v>1861</v>
       </c>
       <c r="F152" s="9" t="str">
-        <f>Base_identifier&amp;C152&amp;"."&amp;E152</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/KeyEntrySet.keyID</v>
       </c>
       <c r="G152" s="9" t="s">
         <v>1943</v>
       </c>
       <c r="H152" s="12" t="str">
-        <f>IF(C152=C151,"","&lt;/table&gt;&lt;h3 id="""&amp;C152&amp;"""&gt;Requirements Class "&amp;C152&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C152&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F152&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G152&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/KeyEntrySet.keyID&lt;br/&gt;&lt;i&gt;The first unsigned short integer in each Key Entry Set SHALL hold the KeyID.&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="153" spans="1:8" ht="30">
+    <row r="153" spans="1:8" ht="45">
       <c r="A153" s="9" t="s">
         <v>4</v>
       </c>
@@ -13766,18 +13770,18 @@
         <v>1864</v>
       </c>
       <c r="F153" s="9" t="str">
-        <f>Base_identifier&amp;C153&amp;"."&amp;E153</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/KeyEntrySet.shortKeyValues</v>
       </c>
       <c r="G153" s="9" t="s">
         <v>2030</v>
       </c>
       <c r="H153" s="12" t="str">
-        <f>IF(C153=C152,"","&lt;/table&gt;&lt;h3 id="""&amp;C153&amp;"""&gt;Requirements Class "&amp;C153&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C153&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F153&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G153&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/KeyEntrySet.shortKeyValues&lt;br/&gt;&lt;i&gt;Following the KeyEntry definitions, the GeoKeyDirectoryTag MAY hold values for keys that are short integers. (NOT CLEAR, maybe the following:  If TIFFTagLocation=0, then Value_Offset contains the actual (SHORT) value of the Key, and Count=1 is implied. shortKeyValues specifies that value. )&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="154" spans="1:8" ht="45">
+    <row r="154" spans="1:8" ht="30">
       <c r="A154" s="9" t="s">
         <v>4</v>
       </c>
@@ -13792,18 +13796,18 @@
         <v>1860</v>
       </c>
       <c r="F154" s="9" t="str">
-        <f>Base_identifier&amp;C154&amp;"."&amp;E154</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/KeyEntrySet.size</v>
       </c>
       <c r="G154" s="9" t="s">
         <v>1944</v>
       </c>
       <c r="H154" s="12" t="str">
-        <f>IF(C154=C153,"","&lt;/table&gt;&lt;h3 id="""&amp;C154&amp;"""&gt;Requirements Class "&amp;C154&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C154&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F154&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G154&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/KeyEntrySet.size&lt;br/&gt;&lt;i&gt;Each Key Entry Set SHALL hold four unsigned short integers&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="155" spans="1:8" ht="30">
+    <row r="155" spans="1:8" ht="45">
       <c r="A155" s="9" t="s">
         <v>4</v>
       </c>
@@ -13818,18 +13822,18 @@
         <v>1862</v>
       </c>
       <c r="F155" s="9" t="str">
-        <f>Base_identifier&amp;C155&amp;"."&amp;E155</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/KeyEntrySet.TIFFTagLocation</v>
       </c>
       <c r="G155" s="9" t="s">
         <v>1945</v>
       </c>
       <c r="H155" s="12" t="str">
-        <f>IF(C155=C154,"","&lt;/table&gt;&lt;h3 id="""&amp;C155&amp;"""&gt;Requirements Class "&amp;C155&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C155&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F155&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G155&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/KeyEntrySet.TIFFTagLocation&lt;br/&gt;&lt;i&gt;The second unsigned short integer in each Key Entry Set SHALL hold the TIFFTagLocation. If TIFFTagLocation is 0, then the value is SHORT, and is contained in the "Value_Offset" entry. Otherwise, the type of the value is implied by the TIFF-Type of the tag containing the value.&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="156" spans="1:8" ht="30">
+    <row r="156" spans="1:8" ht="75">
       <c r="A156" s="9" t="s">
         <v>4</v>
       </c>
@@ -13844,18 +13848,18 @@
         <v>1863</v>
       </c>
       <c r="F156" s="9" t="str">
-        <f>Base_identifier&amp;C156&amp;"."&amp;E156</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/KeyEntrySet.valueOffset</v>
       </c>
       <c r="G156" s="9" t="s">
         <v>2032</v>
       </c>
       <c r="H156" s="12" t="str">
-        <f>IF(C156=C155,"","&lt;/table&gt;&lt;h3 id="""&amp;C156&amp;"""&gt;Requirements Class "&amp;C156&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C156&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F156&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G156&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/KeyEntrySet.valueOffset&lt;br/&gt;&lt;i&gt;The fourth unsigned short integer in each Key Entry Set SHALL hold the Value_Offset. Value_Offset indicates the index-offset *into* the TagArray indicated by TIFFTagLocation, if it is nonzero. If TIFFTagLocation is 0, then Value_Offset contains the actual (SHORT) value of the Key, and Count=1 is implied. Note that the offset is not a byte-offset, but rather an index based on the natural data type of the specified tag array.  &lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="157" spans="1:8" ht="30">
+    <row r="157" spans="1:8" ht="45">
       <c r="A157" s="9" t="s">
         <v>1835</v>
       </c>
@@ -13868,18 +13872,18 @@
         <v>1871</v>
       </c>
       <c r="F157" s="9" t="str">
-        <f>Base_identifier&amp;C157&amp;"."&amp;E157</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/MetadataTag.cardinality</v>
       </c>
       <c r="G157" s="9" t="s">
         <v>21</v>
       </c>
       <c r="H157" s="12" t="str">
-        <f>IF(C157=C156,"","&lt;/table&gt;&lt;h3 id="""&amp;C157&amp;"""&gt;Requirements Class "&amp;C157&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C157&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F157&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G157&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;/table&gt;&lt;h3 id="MetadataTag"&gt;Requirements Class MetadataTag&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/MetadataTag&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/MetadataTag.cardinality&lt;br/&gt;&lt;i&gt;The private TIFF tag for holding XML metadata MAY be used more than once in a single GeoTIFF file.&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="158" spans="1:8" ht="30">
+    <row r="158" spans="1:8" ht="45">
       <c r="A158" s="9" t="s">
         <v>1835</v>
       </c>
@@ -13892,14 +13896,14 @@
         <v>1851</v>
       </c>
       <c r="F158" s="9" t="str">
-        <f>Base_identifier&amp;C158&amp;"."&amp;E158</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/MetadataTag.ID</v>
       </c>
       <c r="G158" s="9" t="s">
         <v>20</v>
       </c>
       <c r="H158" s="12" t="str">
-        <f>IF(C158=C157,"","&lt;/table&gt;&lt;h3 id="""&amp;C158&amp;"""&gt;Requirements Class "&amp;C158&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C158&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F158&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G158&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/MetadataTag.ID&lt;br/&gt;&lt;i&gt;The private TIFF tag for holding XML metadata SHALL have ID=50909&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -13916,14 +13920,14 @@
         <v>1870</v>
       </c>
       <c r="F159" s="9" t="str">
-        <f>Base_identifier&amp;C159&amp;"."&amp;E159</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/MetadataTag.Name</v>
       </c>
       <c r="G159" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H159" s="12" t="str">
-        <f>IF(C159=C158,"","&lt;/table&gt;&lt;h3 id="""&amp;C159&amp;"""&gt;Requirements Class "&amp;C159&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C159&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F159&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G159&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/MetadataTag.Name&lt;br/&gt;&lt;i&gt;The private TIFF tag for holding XML metadata SHALL be named GEO_METADATA&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -13940,14 +13944,14 @@
         <v>1853</v>
       </c>
       <c r="F160" s="9" t="str">
-        <f>Base_identifier&amp;C160&amp;"."&amp;E160</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/ModelPixelScaleTag.count</v>
       </c>
       <c r="G160" s="9" t="s">
         <v>31</v>
       </c>
       <c r="H160" s="12" t="str">
-        <f>IF(C160=C159,"","&lt;/table&gt;&lt;h3 id="""&amp;C160&amp;"""&gt;Requirements Class "&amp;C160&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C160&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F160&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G160&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;/table&gt;&lt;h3 id="ModelPixelScaleTag"&gt;Requirements Class ModelPixelScaleTag&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/ModelPixelScaleTag&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/ModelPixelScaleTag.count&lt;br/&gt;&lt;i&gt;The ModelPixelScaleTag SHALL hold three values (ScaleX, ScaleY, ScaleZ)&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -13964,14 +13968,14 @@
         <v>1853</v>
       </c>
       <c r="F161" s="9" t="str">
-        <f>Base_identifier&amp;C161&amp;"."&amp;E161</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/ModelPixelScaleTag.count</v>
       </c>
       <c r="G161" s="9" t="s">
         <v>31</v>
       </c>
       <c r="H161" s="12" t="str">
-        <f>IF(C161=C160,"","&lt;/table&gt;&lt;h3 id="""&amp;C161&amp;"""&gt;Requirements Class "&amp;C161&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C161&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F161&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G161&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/ModelPixelScaleTag.count&lt;br/&gt;&lt;i&gt;The ModelPixelScaleTag SHALL hold three values (ScaleX, ScaleY, ScaleZ)&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -13988,14 +13992,14 @@
         <v>1851</v>
       </c>
       <c r="F162" s="9" t="str">
-        <f>Base_identifier&amp;C162&amp;"."&amp;E162</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/ModelPixelScaleTag.ID</v>
       </c>
       <c r="G162" s="9" t="s">
         <v>30</v>
       </c>
       <c r="H162" s="12" t="str">
-        <f>IF(C162=C161,"","&lt;/table&gt;&lt;h3 id="""&amp;C162&amp;"""&gt;Requirements Class "&amp;C162&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C162&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F162&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G162&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/ModelPixelScaleTag.ID&lt;br/&gt;&lt;i&gt;The ModelPixelScaleTag SHALL have ID = 33550&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -14012,14 +14016,14 @@
         <v>1874</v>
       </c>
       <c r="F163" s="9" t="str">
-        <f>Base_identifier&amp;C163&amp;"."&amp;E163</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/ModelPixelScaleTag.independent</v>
       </c>
       <c r="G163" s="9" t="s">
         <v>33</v>
       </c>
       <c r="H163" s="12" t="str">
-        <f>IF(C163=C162,"","&lt;/table&gt;&lt;h3 id="""&amp;C163&amp;"""&gt;Requirements Class "&amp;C163&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C163&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F163&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G163&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/ModelPixelScaleTag.independent&lt;br/&gt;&lt;i&gt;The ModelPixelScaleTag SHALL be independent of the Xposition, Yposition, and Orientation TIFF tags&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -14036,14 +14040,14 @@
         <v>1876</v>
       </c>
       <c r="F164" s="9" t="str">
-        <f>Base_identifier&amp;C164&amp;"."&amp;E164</f>
+        <f t="shared" si="8"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/ModelPixelScaleTag.reversal</v>
       </c>
       <c r="G164" s="9" t="s">
         <v>34</v>
       </c>
       <c r="H164" s="12" t="str">
-        <f>IF(C164=C163,"","&lt;/table&gt;&lt;h3 id="""&amp;C164&amp;"""&gt;Requirements Class "&amp;C164&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C164&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F164&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G164&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="9"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/ModelPixelScaleTag.reversal&lt;br/&gt;&lt;i&gt;Negative values of the ModelPixelScaleTag components SHALL indicate simple reversals of orientation between raster and model space (e.g. horizontal or vertical flips)&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -14060,14 +14064,14 @@
         <v>1852</v>
       </c>
       <c r="F165" s="9" t="str">
-        <f>Base_identifier&amp;C165&amp;"."&amp;E165</f>
+        <f t="shared" ref="F165:F196" si="10">Base_identifier&amp;C165&amp;"."&amp;E165</f>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/ModelPixelScaleTag.type</v>
       </c>
       <c r="G165" s="9" t="s">
         <v>29</v>
       </c>
       <c r="H165" s="12" t="str">
-        <f>IF(C165=C164,"","&lt;/table&gt;&lt;h3 id="""&amp;C165&amp;"""&gt;Requirements Class "&amp;C165&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C165&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F165&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G165&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" ref="H165:H196" si="11">IF(C165=C164,"","&lt;/table&gt;&lt;h3 id="""&amp;C165&amp;"""&gt;Requirements Class "&amp;C165&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C165&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F165&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G165&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/ModelPixelScaleTag.type&lt;br/&gt;&lt;i&gt;The ModelPixelScaleTag SHALL have type = DOUBLE&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -14084,14 +14088,14 @@
         <v>1853</v>
       </c>
       <c r="F166" s="9" t="str">
-        <f>Base_identifier&amp;C166&amp;"."&amp;E166</f>
+        <f t="shared" si="10"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/ModelTag.count</v>
       </c>
       <c r="G166" s="9" t="s">
         <v>38</v>
       </c>
       <c r="H166" s="12" t="str">
-        <f>IF(C166=C165,"","&lt;/table&gt;&lt;h3 id="""&amp;C166&amp;"""&gt;Requirements Class "&amp;C166&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C166&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F166&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G166&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="11"/>
         <v>&lt;/table&gt;&lt;h3 id="ModelTag"&gt;Requirements Class ModelTag&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/ModelTag&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/ModelTag.count&lt;br/&gt;&lt;i&gt;If the ModelTiePointTag and ModelPixelScaleTags are defined the ModelTransformationTag SHALL not be used &lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -14108,18 +14112,18 @@
         <v>1853</v>
       </c>
       <c r="F167" s="9" t="str">
-        <f>Base_identifier&amp;C167&amp;"."&amp;E167</f>
+        <f t="shared" si="10"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/ModelTiePointTag.count</v>
       </c>
       <c r="G167" s="9" t="s">
         <v>28</v>
       </c>
       <c r="H167" s="12" t="str">
-        <f>IF(C167=C166,"","&lt;/table&gt;&lt;h3 id="""&amp;C167&amp;"""&gt;Requirements Class "&amp;C167&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C167&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F167&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G167&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="11"/>
         <v>&lt;/table&gt;&lt;h3 id="ModelTiePointTag"&gt;Requirements Class ModelTiePointTag&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/ModelTiePointTag&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/ModelTiePointTag.count&lt;br/&gt;&lt;i&gt;The ModelTiePointTag MAY hold any number of tiepoints&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="30">
+    <row r="168" spans="1:8" ht="45">
       <c r="A168" s="9" t="s">
         <v>1837</v>
       </c>
@@ -14132,14 +14136,14 @@
         <v>1853</v>
       </c>
       <c r="F168" s="9" t="str">
-        <f>Base_identifier&amp;C168&amp;"."&amp;E168</f>
+        <f t="shared" si="10"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/ModelTiePointTag.count</v>
       </c>
       <c r="G168" s="9" t="s">
         <v>1832</v>
       </c>
       <c r="H168" s="12" t="str">
-        <f>IF(C168=C167,"","&lt;/table&gt;&lt;h3 id="""&amp;C168&amp;"""&gt;Requirements Class "&amp;C168&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C168&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F168&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G168&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="11"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/ModelTiePointTag.count&lt;br/&gt;&lt;i&gt;The ModelTiePointTag SHALL only hold one tiepoint that corresponds to the upper left corner of the image.&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -14156,14 +14160,14 @@
         <v>1851</v>
       </c>
       <c r="F169" s="9" t="str">
-        <f>Base_identifier&amp;C169&amp;"."&amp;E169</f>
+        <f t="shared" si="10"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/ModelTiePointTag.ID</v>
       </c>
       <c r="G169" s="9" t="s">
         <v>25</v>
       </c>
       <c r="H169" s="12" t="str">
-        <f>IF(C169=C168,"","&lt;/table&gt;&lt;h3 id="""&amp;C169&amp;"""&gt;Requirements Class "&amp;C169&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C169&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F169&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G169&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="11"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/ModelTiePointTag.ID&lt;br/&gt;&lt;i&gt;The ModelTiePointTag SHALL have ID = 33922&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -14180,18 +14184,18 @@
         <v>1874</v>
       </c>
       <c r="F170" s="9" t="str">
-        <f>Base_identifier&amp;C170&amp;"."&amp;E170</f>
+        <f t="shared" si="10"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/ModelTiePointTag.independent</v>
       </c>
       <c r="G170" s="9" t="s">
         <v>32</v>
       </c>
       <c r="H170" s="12" t="str">
-        <f>IF(C170=C169,"","&lt;/table&gt;&lt;h3 id="""&amp;C170&amp;"""&gt;Requirements Class "&amp;C170&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C170&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F170&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G170&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="11"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/ModelTiePointTag.independent&lt;br/&gt;&lt;i&gt;The ModelTiePointTag SHALL be independent of the Xposition, Yposition, and Orientation TIFF tags&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="171" spans="1:8" ht="45">
+    <row r="171" spans="1:8" ht="30">
       <c r="A171" s="9" t="s">
         <v>24</v>
       </c>
@@ -14204,14 +14208,14 @@
         <v>1860</v>
       </c>
       <c r="F171" s="9" t="str">
-        <f>Base_identifier&amp;C171&amp;"."&amp;E171</f>
+        <f t="shared" si="10"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/ModelTiePointTag.size</v>
       </c>
       <c r="G171" s="9" t="s">
         <v>27</v>
       </c>
       <c r="H171" s="12" t="str">
-        <f>IF(C171=C170,"","&lt;/table&gt;&lt;h3 id="""&amp;C171&amp;"""&gt;Requirements Class "&amp;C171&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C171&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F171&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G171&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="11"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/ModelTiePointTag.size&lt;br/&gt;&lt;i&gt;The ModelTiePointTag SHALL include six values for each tiepoint&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -14228,14 +14232,14 @@
         <v>1852</v>
       </c>
       <c r="F172" s="9" t="str">
-        <f>Base_identifier&amp;C172&amp;"."&amp;E172</f>
+        <f t="shared" si="10"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/ModelTiePointTag.type</v>
       </c>
       <c r="G172" s="9" t="s">
         <v>26</v>
       </c>
       <c r="H172" s="12" t="str">
-        <f>IF(C172=C171,"","&lt;/table&gt;&lt;h3 id="""&amp;C172&amp;"""&gt;Requirements Class "&amp;C172&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C172&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F172&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G172&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="11"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/ModelTiePointTag.type&lt;br/&gt;&lt;i&gt;The ModelTiePointTag SHALL have type = DOUBLE&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -14252,14 +14256,14 @@
         <v>1853</v>
       </c>
       <c r="F173" s="9" t="str">
-        <f>Base_identifier&amp;C173&amp;"."&amp;E173</f>
+        <f t="shared" si="10"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/ModelTransformationTag.count</v>
       </c>
       <c r="G173" s="9" t="s">
         <v>37</v>
       </c>
       <c r="H173" s="12" t="str">
-        <f>IF(C173=C172,"","&lt;/table&gt;&lt;h3 id="""&amp;C173&amp;"""&gt;Requirements Class "&amp;C173&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C173&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F173&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G173&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="11"/>
         <v>&lt;/table&gt;&lt;h3 id="ModelTransformationTag"&gt;Requirements Class ModelTransformationTag&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/ModelTransformationTag&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/ModelTransformationTag.count&lt;br/&gt;&lt;i&gt;The ModelTransformationTag SHALL hold sixteen values &lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -14276,18 +14280,18 @@
         <v>1851</v>
       </c>
       <c r="F174" s="9" t="str">
-        <f>Base_identifier&amp;C174&amp;"."&amp;E174</f>
+        <f t="shared" si="10"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/ModelTransformationTag.ID</v>
       </c>
       <c r="G174" s="9" t="s">
         <v>36</v>
       </c>
       <c r="H174" s="12" t="str">
-        <f>IF(C174=C173,"","&lt;/table&gt;&lt;h3 id="""&amp;C174&amp;"""&gt;Requirements Class "&amp;C174&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C174&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F174&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G174&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="11"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/ModelTransformationTag.ID&lt;br/&gt;&lt;i&gt;The ModelTransformationTag SHALL have ID = 34264&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="175" spans="1:8" ht="30">
+    <row r="175" spans="1:8" ht="45">
       <c r="A175" s="9" t="s">
         <v>1837</v>
       </c>
@@ -14300,14 +14304,14 @@
         <v>1947</v>
       </c>
       <c r="F175" s="9" t="str">
-        <f>Base_identifier&amp;C175&amp;"."&amp;E175</f>
+        <f t="shared" si="10"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/ModelTransformationTag.notAllowed</v>
       </c>
       <c r="G175" s="9" t="s">
         <v>1946</v>
       </c>
       <c r="H175" s="12" t="str">
-        <f>IF(C175=C174,"","&lt;/table&gt;&lt;h3 id="""&amp;C175&amp;"""&gt;Requirements Class "&amp;C175&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C175&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F175&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G175&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="11"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/ModelTransformationTag.notAllowed&lt;br/&gt;&lt;i&gt;The ModelTransformationTag SHALL not be used.&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -14324,14 +14328,14 @@
         <v>1852</v>
       </c>
       <c r="F176" s="9" t="str">
-        <f>Base_identifier&amp;C176&amp;"."&amp;E176</f>
+        <f t="shared" si="10"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/ModelTransformationTag.type</v>
       </c>
       <c r="G176" s="9" t="s">
         <v>35</v>
       </c>
       <c r="H176" s="12" t="str">
-        <f>IF(C176=C175,"","&lt;/table&gt;&lt;h3 id="""&amp;C176&amp;"""&gt;Requirements Class "&amp;C176&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C176&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F176&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G176&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="11"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/ModelTransformationTag.type&lt;br/&gt;&lt;i&gt;The ModelTransformationTag SHALL have type = DOUBLE&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -14348,14 +14352,14 @@
         <v>1851</v>
       </c>
       <c r="F177" s="9" t="str">
-        <f>Base_identifier&amp;C177&amp;"."&amp;E177</f>
+        <f t="shared" si="10"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/VoidAreasTag.ID</v>
       </c>
       <c r="G177" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H177" s="12" t="str">
-        <f>IF(C177=C176,"","&lt;/table&gt;&lt;h3 id="""&amp;C177&amp;"""&gt;Requirements Class "&amp;C177&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C177&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F177&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G177&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="11"/>
         <v>&lt;/table&gt;&lt;h3 id="VoidAreasTag"&gt;Requirements Class VoidAreasTag&lt;/h3&gt;&lt;table border="1" cellpadding="2"&gt;&lt;tr&gt;&lt;td colspan="2" bgcolor="lightgrey"&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan="2"&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VoidAreasTag&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VoidAreasTag.ID&lt;br/&gt;&lt;i&gt;The private TIFF tag for defining void areas SHALL have ID = 42113.&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
@@ -14372,14 +14376,14 @@
         <v>1870</v>
       </c>
       <c r="F178" s="9" t="str">
-        <f>Base_identifier&amp;C178&amp;"."&amp;E178</f>
+        <f t="shared" si="10"/>
         <v>http://www.opengis.net/spec/GeoTIFF/0.0/VoidAreasTag.Name</v>
       </c>
       <c r="G178" s="9" t="s">
         <v>2031</v>
       </c>
       <c r="H178" s="12" t="str">
-        <f>IF(C178=C177,"","&lt;/table&gt;&lt;h3 id="""&amp;C178&amp;"""&gt;Requirements Class "&amp;C178&amp;"&lt;/h3&gt;&lt;table border=""1"" cellpadding=""2""&gt;&lt;tr&gt;&lt;td colspan=""2"" bgcolor=""lightgrey""&gt;&lt;b&gt;Requirements Class&lt;/b&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan=""2""&gt;"&amp;Base_identifier&amp;C178&amp;"&lt;/td&gt;&lt;/tr&gt;")&amp;"&lt;tr&gt;&lt;td bgcolor=""lightgrey""&gt;Requirement&lt;/td&gt;&lt;td&gt;"&amp;F178&amp;"&lt;br/&gt;&lt;i&gt;"&amp;G178&amp;"&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" si="11"/>
         <v>&lt;tr&gt;&lt;td bgcolor="lightgrey"&gt;Requirement&lt;/td&gt;&lt;td&gt;http://www.opengis.net/spec/GeoTIFF/0.0/VoidAreasTag.Name&lt;br/&gt;&lt;i&gt;The private TIFF tag for defining void areas SHALL be named GDAL_NODATA. (GDAL_NODATA is not defined in the GeoTIFF standard, however, this is an private TIFF tag that may be used for the purpose of declaring these values.)&lt;/i&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>

</xml_diff>